<commit_message>
Celestial Dragonblade Meta Update
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/GodwyrmMeta.xlsx
+++ b/Excel_and_CSV/GodwyrmMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E763D82A-B407-4CEB-83AE-05283646E0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48944DA-4AB7-405F-9F49-75578547EA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Archetype Table" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="243">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -739,6 +739,27 @@
   </si>
   <si>
     <t>Reso-Puppet Portal</t>
+  </si>
+  <si>
+    <t>Penguin Guardian</t>
+  </si>
+  <si>
+    <t>7M0qM</t>
+  </si>
+  <si>
+    <t>fskF2</t>
+  </si>
+  <si>
+    <t>Quickblader</t>
+  </si>
+  <si>
+    <t>Kagemitsu, Lost Samurai</t>
+  </si>
+  <si>
+    <t>7M88o</t>
+  </si>
+  <si>
+    <t>5-Hb2</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1067,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1022"/>
+  <dimension ref="A1:I1025"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1382,28 +1403,28 @@
     </row>
     <row r="13" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>214</v>
+      <c r="C13" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>6</v>
+        <v>240</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>6</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1413,122 +1434,122 @@
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>79</v>
+      <c r="C14" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>80</v>
+        <v>242</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>6</v>
+        <v>240</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>6</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="G18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1536,24 +1557,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
+    <row r="19" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>130</v>
+      <c r="C19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>6</v>
@@ -1562,24 +1583,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>57</v>
+    <row r="20" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>103</v>
+      <c r="C20" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
@@ -1588,102 +1609,102 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>92</v>
+    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
@@ -1694,22 +1715,22 @@
     </row>
     <row r="25" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>158</v>
+        <v>59</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>6</v>
@@ -1720,22 +1741,22 @@
     </row>
     <row r="26" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>15</v>
+        <v>152</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>6</v>
@@ -1746,22 +1767,22 @@
     </row>
     <row r="27" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>199</v>
+        <v>127</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>201</v>
+        <v>133</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>200</v>
+        <v>134</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>201</v>
+        <v>58</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>6</v>
@@ -1772,22 +1793,22 @@
     </row>
     <row r="28" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>199</v>
+        <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>6</v>
@@ -1798,22 +1819,22 @@
     </row>
     <row r="29" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>6</v>
@@ -1824,22 +1845,22 @@
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>6</v>
@@ -1850,22 +1871,22 @@
     </row>
     <row r="31" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>175</v>
+        <v>58</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>177</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>6</v>
@@ -1876,126 +1897,126 @@
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>139</v>
+      <c r="C35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>6</v>
@@ -2006,74 +2027,74 @@
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>231</v>
+        <v>116</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>167</v>
+      <c r="C38" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>186</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>187</v>
+        <v>52</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>6</v>
@@ -2084,48 +2105,48 @@
     </row>
     <row r="40" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>179</v>
+        <v>51</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>6</v>
+        <v>234</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>6</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>233</v>
+        <v>187</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>234</v>
+        <v>168</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>6</v>
@@ -2136,22 +2157,22 @@
     </row>
     <row r="42" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>6</v>
@@ -2162,102 +2183,100 @@
     </row>
     <row r="43" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>183</v>
+        <v>82</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>6</v>
@@ -2265,26 +2284,25 @@
       <c r="H46" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>159</v>
+        <v>27</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>6</v>
@@ -2294,123 +2312,126 @@
       </c>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="G51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>67</v>
@@ -2425,24 +2446,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>6</v>
@@ -2451,24 +2472,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>204</v>
+        <v>31</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>206</v>
+        <v>62</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>205</v>
+        <v>63</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>6</v>
@@ -2477,154 +2498,154 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>204</v>
+        <v>64</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D57" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="G58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>6</v>
@@ -2633,104 +2654,161 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="H61" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="H62" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C63" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
+      <c r="G66" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -2753,16 +2831,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-    </row>
+    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
@@ -2783,22 +2852,43 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+    </row>
     <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="7"/>
-    </row>
-    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="7"/>
-    </row>
-    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B82" s="7"/>
-    </row>
+    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="83" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B83" s="7"/>
     </row>
@@ -5618,6 +5708,15 @@
     </row>
     <row r="1022" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1022" s="7"/>
+    </row>
+    <row r="1023" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1023" s="7"/>
+    </row>
+    <row r="1024" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1024" s="7"/>
+    </row>
+    <row r="1025" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1025" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5629,7 +5728,7 @@
           <x14:formula1>
             <xm:f>Class!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B80:B1022 B68:B72 J58:J60 R58:R60 Z58:Z60 AH58:AH60 AP58:AP60 AX58:AX60 BF58:BF60 BN58:BN60 BV58:BV60 CD58:CD60 CL58:CL60 CT58:CT60 DB58:DB60 DJ58:DJ60 DR58:DR60 DZ58:DZ60 EH58:EH60 EP58:EP60 EX58:EX60 FF58:FF60 FN58:FN60 FV58:FV60 GD58:GD60 GL58:GL60 GT58:GT60 HB58:HB60 HJ58:HJ60 HR58:HR60 HZ58:HZ60 IH58:IH60 IP58:IP60 IX58:IX60 JF58:JF60 JN58:JN60 JV58:JV60 KD58:KD60 KL58:KL60 KT58:KT60 LB58:LB60 LJ58:LJ60 LR58:LR60 LZ58:LZ60 MH58:MH60 MP58:MP60 MX58:MX60 NF58:NF60 NN58:NN60 NV58:NV60 OD58:OD60 OL58:OL60 OT58:OT60 PB58:PB60 PJ58:PJ60 PR58:PR60 PZ58:PZ60 QH58:QH60 QP58:QP60 QX58:QX60 RF58:RF60 RN58:RN60 RV58:RV60 SD58:SD60 SL58:SL60 ST58:ST60 TB58:TB60 TJ58:TJ60 TR58:TR60 TZ58:TZ60 UH58:UH60 UP58:UP60 UX58:UX60 VF58:VF60 VN58:VN60 VV58:VV60 WD58:WD60 WL58:WL60 WT58:WT60 XB58:XB60 XJ58:XJ60 XR58:XR60 XZ58:XZ60 YH58:YH60 YP58:YP60 YX58:YX60 ZF58:ZF60 ZN58:ZN60 ZV58:ZV60 AAD58:AAD60 AAL58:AAL60 AAT58:AAT60 ABB58:ABB60 ABJ58:ABJ60 ABR58:ABR60 ABZ58:ABZ60 ACH58:ACH60 ACP58:ACP60 ACX58:ACX60 ADF58:ADF60 ADN58:ADN60 ADV58:ADV60 AED58:AED60 AEL58:AEL60 AET58:AET60 AFB58:AFB60 AFJ58:AFJ60 AFR58:AFR60 AFZ58:AFZ60 AGH58:AGH60 AGP58:AGP60 AGX58:AGX60 AHF58:AHF60 AHN58:AHN60 AHV58:AHV60 AID58:AID60 AIL58:AIL60 AIT58:AIT60 AJB58:AJB60 AJJ58:AJJ60 AJR58:AJR60 AJZ58:AJZ60 AKH58:AKH60 AKP58:AKP60 AKX58:AKX60 ALF58:ALF60 ALN58:ALN60 ALV58:ALV60 AMD58:AMD60 AML58:AML60 AMT58:AMT60 ANB58:ANB60 ANJ58:ANJ60 ANR58:ANR60 ANZ58:ANZ60 AOH58:AOH60 AOP58:AOP60 AOX58:AOX60 APF58:APF60 APN58:APN60 APV58:APV60 AQD58:AQD60 AQL58:AQL60 AQT58:AQT60 ARB58:ARB60 ARJ58:ARJ60 ARR58:ARR60 ARZ58:ARZ60 ASH58:ASH60 ASP58:ASP60 ASX58:ASX60 ATF58:ATF60 ATN58:ATN60 ATV58:ATV60 AUD58:AUD60 AUL58:AUL60 AUT58:AUT60 AVB58:AVB60 AVJ58:AVJ60 AVR58:AVR60 AVZ58:AVZ60 AWH58:AWH60 AWP58:AWP60 AWX58:AWX60 AXF58:AXF60 AXN58:AXN60 AXV58:AXV60 AYD58:AYD60 AYL58:AYL60 AYT58:AYT60 AZB58:AZB60 AZJ58:AZJ60 AZR58:AZR60 AZZ58:AZZ60 BAH58:BAH60 BAP58:BAP60 BAX58:BAX60 BBF58:BBF60 BBN58:BBN60 BBV58:BBV60 BCD58:BCD60 BCL58:BCL60 BCT58:BCT60 BDB58:BDB60 BDJ58:BDJ60 BDR58:BDR60 BDZ58:BDZ60 BEH58:BEH60 BEP58:BEP60 BEX58:BEX60 BFF58:BFF60 BFN58:BFN60 BFV58:BFV60 BGD58:BGD60 BGL58:BGL60 BGT58:BGT60 BHB58:BHB60 BHJ58:BHJ60 BHR58:BHR60 BHZ58:BHZ60 BIH58:BIH60 BIP58:BIP60 BIX58:BIX60 BJF58:BJF60 BJN58:BJN60 BJV58:BJV60 BKD58:BKD60 BKL58:BKL60 BKT58:BKT60 BLB58:BLB60 BLJ58:BLJ60 BLR58:BLR60 BLZ58:BLZ60 BMH58:BMH60 BMP58:BMP60 BMX58:BMX60 BNF58:BNF60 BNN58:BNN60 BNV58:BNV60 BOD58:BOD60 BOL58:BOL60 BOT58:BOT60 BPB58:BPB60 BPJ58:BPJ60 BPR58:BPR60 BPZ58:BPZ60 BQH58:BQH60 BQP58:BQP60 BQX58:BQX60 BRF58:BRF60 BRN58:BRN60 BRV58:BRV60 BSD58:BSD60 BSL58:BSL60 BST58:BST60 BTB58:BTB60 BTJ58:BTJ60 BTR58:BTR60 BTZ58:BTZ60 BUH58:BUH60 BUP58:BUP60 BUX58:BUX60 BVF58:BVF60 BVN58:BVN60 BVV58:BVV60 BWD58:BWD60 BWL58:BWL60 BWT58:BWT60 BXB58:BXB60 BXJ58:BXJ60 BXR58:BXR60 BXZ58:BXZ60 BYH58:BYH60 BYP58:BYP60 BYX58:BYX60 BZF58:BZF60 BZN58:BZN60 BZV58:BZV60 CAD58:CAD60 CAL58:CAL60 CAT58:CAT60 CBB58:CBB60 CBJ58:CBJ60 CBR58:CBR60 CBZ58:CBZ60 CCH58:CCH60 CCP58:CCP60 CCX58:CCX60 CDF58:CDF60 CDN58:CDN60 CDV58:CDV60 CED58:CED60 CEL58:CEL60 CET58:CET60 CFB58:CFB60 CFJ58:CFJ60 CFR58:CFR60 CFZ58:CFZ60 CGH58:CGH60 CGP58:CGP60 CGX58:CGX60 CHF58:CHF60 CHN58:CHN60 CHV58:CHV60 CID58:CID60 CIL58:CIL60 CIT58:CIT60 CJB58:CJB60 CJJ58:CJJ60 CJR58:CJR60 CJZ58:CJZ60 CKH58:CKH60 CKP58:CKP60 CKX58:CKX60 CLF58:CLF60 CLN58:CLN60 CLV58:CLV60 CMD58:CMD60 CML58:CML60 CMT58:CMT60 CNB58:CNB60 CNJ58:CNJ60 CNR58:CNR60 CNZ58:CNZ60 COH58:COH60 COP58:COP60 COX58:COX60 CPF58:CPF60 CPN58:CPN60 CPV58:CPV60 CQD58:CQD60 CQL58:CQL60 CQT58:CQT60 CRB58:CRB60 CRJ58:CRJ60 CRR58:CRR60 CRZ58:CRZ60 CSH58:CSH60 CSP58:CSP60 CSX58:CSX60 CTF58:CTF60 CTN58:CTN60 CTV58:CTV60 CUD58:CUD60 CUL58:CUL60 CUT58:CUT60 CVB58:CVB60 CVJ58:CVJ60 CVR58:CVR60 CVZ58:CVZ60 CWH58:CWH60 CWP58:CWP60 CWX58:CWX60 CXF58:CXF60 CXN58:CXN60 CXV58:CXV60 CYD58:CYD60 CYL58:CYL60 CYT58:CYT60 CZB58:CZB60 CZJ58:CZJ60 CZR58:CZR60 CZZ58:CZZ60 DAH58:DAH60 DAP58:DAP60 DAX58:DAX60 DBF58:DBF60 DBN58:DBN60 DBV58:DBV60 DCD58:DCD60 DCL58:DCL60 DCT58:DCT60 DDB58:DDB60 DDJ58:DDJ60 DDR58:DDR60 DDZ58:DDZ60 DEH58:DEH60 DEP58:DEP60 DEX58:DEX60 DFF58:DFF60 DFN58:DFN60 DFV58:DFV60 DGD58:DGD60 DGL58:DGL60 DGT58:DGT60 DHB58:DHB60 DHJ58:DHJ60 DHR58:DHR60 DHZ58:DHZ60 DIH58:DIH60 DIP58:DIP60 DIX58:DIX60 DJF58:DJF60 DJN58:DJN60 DJV58:DJV60 DKD58:DKD60 DKL58:DKL60 DKT58:DKT60 DLB58:DLB60 DLJ58:DLJ60 DLR58:DLR60 DLZ58:DLZ60 DMH58:DMH60 DMP58:DMP60 DMX58:DMX60 DNF58:DNF60 DNN58:DNN60 DNV58:DNV60 DOD58:DOD60 DOL58:DOL60 DOT58:DOT60 DPB58:DPB60 DPJ58:DPJ60 DPR58:DPR60 DPZ58:DPZ60 DQH58:DQH60 DQP58:DQP60 DQX58:DQX60 DRF58:DRF60 DRN58:DRN60 DRV58:DRV60 DSD58:DSD60 DSL58:DSL60 DST58:DST60 DTB58:DTB60 DTJ58:DTJ60 DTR58:DTR60 DTZ58:DTZ60 DUH58:DUH60 DUP58:DUP60 DUX58:DUX60 DVF58:DVF60 DVN58:DVN60 DVV58:DVV60 DWD58:DWD60 DWL58:DWL60 DWT58:DWT60 DXB58:DXB60 DXJ58:DXJ60 DXR58:DXR60 DXZ58:DXZ60 DYH58:DYH60 DYP58:DYP60 DYX58:DYX60 DZF58:DZF60 DZN58:DZN60 DZV58:DZV60 EAD58:EAD60 EAL58:EAL60 EAT58:EAT60 EBB58:EBB60 EBJ58:EBJ60 EBR58:EBR60 EBZ58:EBZ60 ECH58:ECH60 ECP58:ECP60 ECX58:ECX60 EDF58:EDF60 EDN58:EDN60 EDV58:EDV60 EED58:EED60 EEL58:EEL60 EET58:EET60 EFB58:EFB60 EFJ58:EFJ60 EFR58:EFR60 EFZ58:EFZ60 EGH58:EGH60 EGP58:EGP60 EGX58:EGX60 EHF58:EHF60 EHN58:EHN60 EHV58:EHV60 EID58:EID60 EIL58:EIL60 EIT58:EIT60 EJB58:EJB60 EJJ58:EJJ60 EJR58:EJR60 EJZ58:EJZ60 EKH58:EKH60 EKP58:EKP60 EKX58:EKX60 ELF58:ELF60 ELN58:ELN60 ELV58:ELV60 EMD58:EMD60 EML58:EML60 EMT58:EMT60 ENB58:ENB60 ENJ58:ENJ60 ENR58:ENR60 ENZ58:ENZ60 EOH58:EOH60 EOP58:EOP60 EOX58:EOX60 EPF58:EPF60 EPN58:EPN60 EPV58:EPV60 EQD58:EQD60 EQL58:EQL60 EQT58:EQT60 ERB58:ERB60 ERJ58:ERJ60 ERR58:ERR60 ERZ58:ERZ60 ESH58:ESH60 ESP58:ESP60 ESX58:ESX60 ETF58:ETF60 ETN58:ETN60 ETV58:ETV60 EUD58:EUD60 EUL58:EUL60 EUT58:EUT60 EVB58:EVB60 EVJ58:EVJ60 EVR58:EVR60 EVZ58:EVZ60 EWH58:EWH60 EWP58:EWP60 EWX58:EWX60 EXF58:EXF60 EXN58:EXN60 EXV58:EXV60 EYD58:EYD60 EYL58:EYL60 EYT58:EYT60 EZB58:EZB60 EZJ58:EZJ60 EZR58:EZR60 EZZ58:EZZ60 FAH58:FAH60 FAP58:FAP60 FAX58:FAX60 FBF58:FBF60 FBN58:FBN60 FBV58:FBV60 FCD58:FCD60 FCL58:FCL60 FCT58:FCT60 FDB58:FDB60 FDJ58:FDJ60 FDR58:FDR60 FDZ58:FDZ60 FEH58:FEH60 FEP58:FEP60 FEX58:FEX60 FFF58:FFF60 FFN58:FFN60 FFV58:FFV60 FGD58:FGD60 FGL58:FGL60 FGT58:FGT60 FHB58:FHB60 FHJ58:FHJ60 FHR58:FHR60 FHZ58:FHZ60 FIH58:FIH60 FIP58:FIP60 FIX58:FIX60 FJF58:FJF60 FJN58:FJN60 FJV58:FJV60 FKD58:FKD60 FKL58:FKL60 FKT58:FKT60 FLB58:FLB60 FLJ58:FLJ60 FLR58:FLR60 FLZ58:FLZ60 FMH58:FMH60 FMP58:FMP60 FMX58:FMX60 FNF58:FNF60 FNN58:FNN60 FNV58:FNV60 FOD58:FOD60 FOL58:FOL60 FOT58:FOT60 FPB58:FPB60 FPJ58:FPJ60 FPR58:FPR60 FPZ58:FPZ60 FQH58:FQH60 FQP58:FQP60 FQX58:FQX60 FRF58:FRF60 FRN58:FRN60 FRV58:FRV60 FSD58:FSD60 FSL58:FSL60 FST58:FST60 FTB58:FTB60 FTJ58:FTJ60 FTR58:FTR60 FTZ58:FTZ60 FUH58:FUH60 FUP58:FUP60 FUX58:FUX60 FVF58:FVF60 FVN58:FVN60 FVV58:FVV60 FWD58:FWD60 FWL58:FWL60 FWT58:FWT60 FXB58:FXB60 FXJ58:FXJ60 FXR58:FXR60 FXZ58:FXZ60 FYH58:FYH60 FYP58:FYP60 FYX58:FYX60 FZF58:FZF60 FZN58:FZN60 FZV58:FZV60 GAD58:GAD60 GAL58:GAL60 GAT58:GAT60 GBB58:GBB60 GBJ58:GBJ60 GBR58:GBR60 GBZ58:GBZ60 GCH58:GCH60 GCP58:GCP60 GCX58:GCX60 GDF58:GDF60 GDN58:GDN60 GDV58:GDV60 GED58:GED60 GEL58:GEL60 GET58:GET60 GFB58:GFB60 GFJ58:GFJ60 GFR58:GFR60 GFZ58:GFZ60 GGH58:GGH60 GGP58:GGP60 GGX58:GGX60 GHF58:GHF60 GHN58:GHN60 GHV58:GHV60 GID58:GID60 GIL58:GIL60 GIT58:GIT60 GJB58:GJB60 GJJ58:GJJ60 GJR58:GJR60 GJZ58:GJZ60 GKH58:GKH60 GKP58:GKP60 GKX58:GKX60 GLF58:GLF60 GLN58:GLN60 GLV58:GLV60 GMD58:GMD60 GML58:GML60 GMT58:GMT60 GNB58:GNB60 GNJ58:GNJ60 GNR58:GNR60 GNZ58:GNZ60 GOH58:GOH60 GOP58:GOP60 GOX58:GOX60 GPF58:GPF60 GPN58:GPN60 GPV58:GPV60 GQD58:GQD60 GQL58:GQL60 GQT58:GQT60 GRB58:GRB60 GRJ58:GRJ60 GRR58:GRR60 GRZ58:GRZ60 GSH58:GSH60 GSP58:GSP60 GSX58:GSX60 GTF58:GTF60 GTN58:GTN60 GTV58:GTV60 GUD58:GUD60 GUL58:GUL60 GUT58:GUT60 GVB58:GVB60 GVJ58:GVJ60 GVR58:GVR60 GVZ58:GVZ60 GWH58:GWH60 GWP58:GWP60 GWX58:GWX60 GXF58:GXF60 GXN58:GXN60 GXV58:GXV60 GYD58:GYD60 GYL58:GYL60 GYT58:GYT60 GZB58:GZB60 GZJ58:GZJ60 GZR58:GZR60 GZZ58:GZZ60 HAH58:HAH60 HAP58:HAP60 HAX58:HAX60 HBF58:HBF60 HBN58:HBN60 HBV58:HBV60 HCD58:HCD60 HCL58:HCL60 HCT58:HCT60 HDB58:HDB60 HDJ58:HDJ60 HDR58:HDR60 HDZ58:HDZ60 HEH58:HEH60 HEP58:HEP60 HEX58:HEX60 HFF58:HFF60 HFN58:HFN60 HFV58:HFV60 HGD58:HGD60 HGL58:HGL60 HGT58:HGT60 HHB58:HHB60 HHJ58:HHJ60 HHR58:HHR60 HHZ58:HHZ60 HIH58:HIH60 HIP58:HIP60 HIX58:HIX60 HJF58:HJF60 HJN58:HJN60 HJV58:HJV60 HKD58:HKD60 HKL58:HKL60 HKT58:HKT60 HLB58:HLB60 HLJ58:HLJ60 HLR58:HLR60 HLZ58:HLZ60 HMH58:HMH60 HMP58:HMP60 HMX58:HMX60 HNF58:HNF60 HNN58:HNN60 HNV58:HNV60 HOD58:HOD60 HOL58:HOL60 HOT58:HOT60 HPB58:HPB60 HPJ58:HPJ60 HPR58:HPR60 HPZ58:HPZ60 HQH58:HQH60 HQP58:HQP60 HQX58:HQX60 HRF58:HRF60 HRN58:HRN60 HRV58:HRV60 HSD58:HSD60 HSL58:HSL60 HST58:HST60 HTB58:HTB60 HTJ58:HTJ60 HTR58:HTR60 HTZ58:HTZ60 HUH58:HUH60 HUP58:HUP60 HUX58:HUX60 HVF58:HVF60 HVN58:HVN60 HVV58:HVV60 HWD58:HWD60 HWL58:HWL60 HWT58:HWT60 HXB58:HXB60 HXJ58:HXJ60 HXR58:HXR60 HXZ58:HXZ60 HYH58:HYH60 HYP58:HYP60 HYX58:HYX60 HZF58:HZF60 HZN58:HZN60 HZV58:HZV60 IAD58:IAD60 IAL58:IAL60 IAT58:IAT60 IBB58:IBB60 IBJ58:IBJ60 IBR58:IBR60 IBZ58:IBZ60 ICH58:ICH60 ICP58:ICP60 ICX58:ICX60 IDF58:IDF60 IDN58:IDN60 IDV58:IDV60 IED58:IED60 IEL58:IEL60 IET58:IET60 IFB58:IFB60 IFJ58:IFJ60 IFR58:IFR60 IFZ58:IFZ60 IGH58:IGH60 IGP58:IGP60 IGX58:IGX60 IHF58:IHF60 IHN58:IHN60 IHV58:IHV60 IID58:IID60 IIL58:IIL60 IIT58:IIT60 IJB58:IJB60 IJJ58:IJJ60 IJR58:IJR60 IJZ58:IJZ60 IKH58:IKH60 IKP58:IKP60 IKX58:IKX60 ILF58:ILF60 ILN58:ILN60 ILV58:ILV60 IMD58:IMD60 IML58:IML60 IMT58:IMT60 INB58:INB60 INJ58:INJ60 INR58:INR60 INZ58:INZ60 IOH58:IOH60 IOP58:IOP60 IOX58:IOX60 IPF58:IPF60 IPN58:IPN60 IPV58:IPV60 IQD58:IQD60 IQL58:IQL60 IQT58:IQT60 IRB58:IRB60 IRJ58:IRJ60 IRR58:IRR60 IRZ58:IRZ60 ISH58:ISH60 ISP58:ISP60 ISX58:ISX60 ITF58:ITF60 ITN58:ITN60 ITV58:ITV60 IUD58:IUD60 IUL58:IUL60 IUT58:IUT60 IVB58:IVB60 IVJ58:IVJ60 IVR58:IVR60 IVZ58:IVZ60 IWH58:IWH60 IWP58:IWP60 IWX58:IWX60 IXF58:IXF60 IXN58:IXN60 IXV58:IXV60 IYD58:IYD60 IYL58:IYL60 IYT58:IYT60 IZB58:IZB60 IZJ58:IZJ60 IZR58:IZR60 IZZ58:IZZ60 JAH58:JAH60 JAP58:JAP60 JAX58:JAX60 JBF58:JBF60 JBN58:JBN60 JBV58:JBV60 JCD58:JCD60 JCL58:JCL60 JCT58:JCT60 JDB58:JDB60 JDJ58:JDJ60 JDR58:JDR60 JDZ58:JDZ60 JEH58:JEH60 JEP58:JEP60 JEX58:JEX60 JFF58:JFF60 JFN58:JFN60 JFV58:JFV60 JGD58:JGD60 JGL58:JGL60 JGT58:JGT60 JHB58:JHB60 JHJ58:JHJ60 JHR58:JHR60 JHZ58:JHZ60 JIH58:JIH60 JIP58:JIP60 JIX58:JIX60 JJF58:JJF60 JJN58:JJN60 JJV58:JJV60 JKD58:JKD60 JKL58:JKL60 JKT58:JKT60 JLB58:JLB60 JLJ58:JLJ60 JLR58:JLR60 JLZ58:JLZ60 JMH58:JMH60 JMP58:JMP60 JMX58:JMX60 JNF58:JNF60 JNN58:JNN60 JNV58:JNV60 JOD58:JOD60 JOL58:JOL60 JOT58:JOT60 JPB58:JPB60 JPJ58:JPJ60 JPR58:JPR60 JPZ58:JPZ60 JQH58:JQH60 JQP58:JQP60 JQX58:JQX60 JRF58:JRF60 JRN58:JRN60 JRV58:JRV60 JSD58:JSD60 JSL58:JSL60 JST58:JST60 JTB58:JTB60 JTJ58:JTJ60 JTR58:JTR60 JTZ58:JTZ60 JUH58:JUH60 JUP58:JUP60 JUX58:JUX60 JVF58:JVF60 JVN58:JVN60 JVV58:JVV60 JWD58:JWD60 JWL58:JWL60 JWT58:JWT60 JXB58:JXB60 JXJ58:JXJ60 JXR58:JXR60 JXZ58:JXZ60 JYH58:JYH60 JYP58:JYP60 JYX58:JYX60 JZF58:JZF60 JZN58:JZN60 JZV58:JZV60 KAD58:KAD60 KAL58:KAL60 KAT58:KAT60 KBB58:KBB60 KBJ58:KBJ60 KBR58:KBR60 KBZ58:KBZ60 KCH58:KCH60 KCP58:KCP60 KCX58:KCX60 KDF58:KDF60 KDN58:KDN60 KDV58:KDV60 KED58:KED60 KEL58:KEL60 KET58:KET60 KFB58:KFB60 KFJ58:KFJ60 KFR58:KFR60 KFZ58:KFZ60 KGH58:KGH60 KGP58:KGP60 KGX58:KGX60 KHF58:KHF60 KHN58:KHN60 KHV58:KHV60 KID58:KID60 KIL58:KIL60 KIT58:KIT60 KJB58:KJB60 KJJ58:KJJ60 KJR58:KJR60 KJZ58:KJZ60 KKH58:KKH60 KKP58:KKP60 KKX58:KKX60 KLF58:KLF60 KLN58:KLN60 KLV58:KLV60 KMD58:KMD60 KML58:KML60 KMT58:KMT60 KNB58:KNB60 KNJ58:KNJ60 KNR58:KNR60 KNZ58:KNZ60 KOH58:KOH60 KOP58:KOP60 KOX58:KOX60 KPF58:KPF60 KPN58:KPN60 KPV58:KPV60 KQD58:KQD60 KQL58:KQL60 KQT58:KQT60 KRB58:KRB60 KRJ58:KRJ60 KRR58:KRR60 KRZ58:KRZ60 KSH58:KSH60 KSP58:KSP60 KSX58:KSX60 KTF58:KTF60 KTN58:KTN60 KTV58:KTV60 KUD58:KUD60 KUL58:KUL60 KUT58:KUT60 KVB58:KVB60 KVJ58:KVJ60 KVR58:KVR60 KVZ58:KVZ60 KWH58:KWH60 KWP58:KWP60 KWX58:KWX60 KXF58:KXF60 KXN58:KXN60 KXV58:KXV60 KYD58:KYD60 KYL58:KYL60 KYT58:KYT60 KZB58:KZB60 KZJ58:KZJ60 KZR58:KZR60 KZZ58:KZZ60 LAH58:LAH60 LAP58:LAP60 LAX58:LAX60 LBF58:LBF60 LBN58:LBN60 LBV58:LBV60 LCD58:LCD60 LCL58:LCL60 LCT58:LCT60 LDB58:LDB60 LDJ58:LDJ60 LDR58:LDR60 LDZ58:LDZ60 LEH58:LEH60 LEP58:LEP60 LEX58:LEX60 LFF58:LFF60 LFN58:LFN60 LFV58:LFV60 LGD58:LGD60 LGL58:LGL60 LGT58:LGT60 LHB58:LHB60 LHJ58:LHJ60 LHR58:LHR60 LHZ58:LHZ60 LIH58:LIH60 LIP58:LIP60 LIX58:LIX60 LJF58:LJF60 LJN58:LJN60 LJV58:LJV60 LKD58:LKD60 LKL58:LKL60 LKT58:LKT60 LLB58:LLB60 LLJ58:LLJ60 LLR58:LLR60 LLZ58:LLZ60 LMH58:LMH60 LMP58:LMP60 LMX58:LMX60 LNF58:LNF60 LNN58:LNN60 LNV58:LNV60 LOD58:LOD60 LOL58:LOL60 LOT58:LOT60 LPB58:LPB60 LPJ58:LPJ60 LPR58:LPR60 LPZ58:LPZ60 LQH58:LQH60 LQP58:LQP60 LQX58:LQX60 LRF58:LRF60 LRN58:LRN60 LRV58:LRV60 LSD58:LSD60 LSL58:LSL60 LST58:LST60 LTB58:LTB60 LTJ58:LTJ60 LTR58:LTR60 LTZ58:LTZ60 LUH58:LUH60 LUP58:LUP60 LUX58:LUX60 LVF58:LVF60 LVN58:LVN60 LVV58:LVV60 LWD58:LWD60 LWL58:LWL60 LWT58:LWT60 LXB58:LXB60 LXJ58:LXJ60 LXR58:LXR60 LXZ58:LXZ60 LYH58:LYH60 LYP58:LYP60 LYX58:LYX60 LZF58:LZF60 LZN58:LZN60 LZV58:LZV60 MAD58:MAD60 MAL58:MAL60 MAT58:MAT60 MBB58:MBB60 MBJ58:MBJ60 MBR58:MBR60 MBZ58:MBZ60 MCH58:MCH60 MCP58:MCP60 MCX58:MCX60 MDF58:MDF60 MDN58:MDN60 MDV58:MDV60 MED58:MED60 MEL58:MEL60 MET58:MET60 MFB58:MFB60 MFJ58:MFJ60 MFR58:MFR60 MFZ58:MFZ60 MGH58:MGH60 MGP58:MGP60 MGX58:MGX60 MHF58:MHF60 MHN58:MHN60 MHV58:MHV60 MID58:MID60 MIL58:MIL60 MIT58:MIT60 MJB58:MJB60 MJJ58:MJJ60 MJR58:MJR60 MJZ58:MJZ60 MKH58:MKH60 MKP58:MKP60 MKX58:MKX60 MLF58:MLF60 MLN58:MLN60 MLV58:MLV60 MMD58:MMD60 MML58:MML60 MMT58:MMT60 MNB58:MNB60 MNJ58:MNJ60 MNR58:MNR60 MNZ58:MNZ60 MOH58:MOH60 MOP58:MOP60 MOX58:MOX60 MPF58:MPF60 MPN58:MPN60 MPV58:MPV60 MQD58:MQD60 MQL58:MQL60 MQT58:MQT60 MRB58:MRB60 MRJ58:MRJ60 MRR58:MRR60 MRZ58:MRZ60 MSH58:MSH60 MSP58:MSP60 MSX58:MSX60 MTF58:MTF60 MTN58:MTN60 MTV58:MTV60 MUD58:MUD60 MUL58:MUL60 MUT58:MUT60 MVB58:MVB60 MVJ58:MVJ60 MVR58:MVR60 MVZ58:MVZ60 MWH58:MWH60 MWP58:MWP60 MWX58:MWX60 MXF58:MXF60 MXN58:MXN60 MXV58:MXV60 MYD58:MYD60 MYL58:MYL60 MYT58:MYT60 MZB58:MZB60 MZJ58:MZJ60 MZR58:MZR60 MZZ58:MZZ60 NAH58:NAH60 NAP58:NAP60 NAX58:NAX60 NBF58:NBF60 NBN58:NBN60 NBV58:NBV60 NCD58:NCD60 NCL58:NCL60 NCT58:NCT60 NDB58:NDB60 NDJ58:NDJ60 NDR58:NDR60 NDZ58:NDZ60 NEH58:NEH60 NEP58:NEP60 NEX58:NEX60 NFF58:NFF60 NFN58:NFN60 NFV58:NFV60 NGD58:NGD60 NGL58:NGL60 NGT58:NGT60 NHB58:NHB60 NHJ58:NHJ60 NHR58:NHR60 NHZ58:NHZ60 NIH58:NIH60 NIP58:NIP60 NIX58:NIX60 NJF58:NJF60 NJN58:NJN60 NJV58:NJV60 NKD58:NKD60 NKL58:NKL60 NKT58:NKT60 NLB58:NLB60 NLJ58:NLJ60 NLR58:NLR60 NLZ58:NLZ60 NMH58:NMH60 NMP58:NMP60 NMX58:NMX60 NNF58:NNF60 NNN58:NNN60 NNV58:NNV60 NOD58:NOD60 NOL58:NOL60 NOT58:NOT60 NPB58:NPB60 NPJ58:NPJ60 NPR58:NPR60 NPZ58:NPZ60 NQH58:NQH60 NQP58:NQP60 NQX58:NQX60 NRF58:NRF60 NRN58:NRN60 NRV58:NRV60 NSD58:NSD60 NSL58:NSL60 NST58:NST60 NTB58:NTB60 NTJ58:NTJ60 NTR58:NTR60 NTZ58:NTZ60 NUH58:NUH60 NUP58:NUP60 NUX58:NUX60 NVF58:NVF60 NVN58:NVN60 NVV58:NVV60 NWD58:NWD60 NWL58:NWL60 NWT58:NWT60 NXB58:NXB60 NXJ58:NXJ60 NXR58:NXR60 NXZ58:NXZ60 NYH58:NYH60 NYP58:NYP60 NYX58:NYX60 NZF58:NZF60 NZN58:NZN60 NZV58:NZV60 OAD58:OAD60 OAL58:OAL60 OAT58:OAT60 OBB58:OBB60 OBJ58:OBJ60 OBR58:OBR60 OBZ58:OBZ60 OCH58:OCH60 OCP58:OCP60 OCX58:OCX60 ODF58:ODF60 ODN58:ODN60 ODV58:ODV60 OED58:OED60 OEL58:OEL60 OET58:OET60 OFB58:OFB60 OFJ58:OFJ60 OFR58:OFR60 OFZ58:OFZ60 OGH58:OGH60 OGP58:OGP60 OGX58:OGX60 OHF58:OHF60 OHN58:OHN60 OHV58:OHV60 OID58:OID60 OIL58:OIL60 OIT58:OIT60 OJB58:OJB60 OJJ58:OJJ60 OJR58:OJR60 OJZ58:OJZ60 OKH58:OKH60 OKP58:OKP60 OKX58:OKX60 OLF58:OLF60 OLN58:OLN60 OLV58:OLV60 OMD58:OMD60 OML58:OML60 OMT58:OMT60 ONB58:ONB60 ONJ58:ONJ60 ONR58:ONR60 ONZ58:ONZ60 OOH58:OOH60 OOP58:OOP60 OOX58:OOX60 OPF58:OPF60 OPN58:OPN60 OPV58:OPV60 OQD58:OQD60 OQL58:OQL60 OQT58:OQT60 ORB58:ORB60 ORJ58:ORJ60 ORR58:ORR60 ORZ58:ORZ60 OSH58:OSH60 OSP58:OSP60 OSX58:OSX60 OTF58:OTF60 OTN58:OTN60 OTV58:OTV60 OUD58:OUD60 OUL58:OUL60 OUT58:OUT60 OVB58:OVB60 OVJ58:OVJ60 OVR58:OVR60 OVZ58:OVZ60 OWH58:OWH60 OWP58:OWP60 OWX58:OWX60 OXF58:OXF60 OXN58:OXN60 OXV58:OXV60 OYD58:OYD60 OYL58:OYL60 OYT58:OYT60 OZB58:OZB60 OZJ58:OZJ60 OZR58:OZR60 OZZ58:OZZ60 PAH58:PAH60 PAP58:PAP60 PAX58:PAX60 PBF58:PBF60 PBN58:PBN60 PBV58:PBV60 PCD58:PCD60 PCL58:PCL60 PCT58:PCT60 PDB58:PDB60 PDJ58:PDJ60 PDR58:PDR60 PDZ58:PDZ60 PEH58:PEH60 PEP58:PEP60 PEX58:PEX60 PFF58:PFF60 PFN58:PFN60 PFV58:PFV60 PGD58:PGD60 PGL58:PGL60 PGT58:PGT60 PHB58:PHB60 PHJ58:PHJ60 PHR58:PHR60 PHZ58:PHZ60 PIH58:PIH60 PIP58:PIP60 PIX58:PIX60 PJF58:PJF60 PJN58:PJN60 PJV58:PJV60 PKD58:PKD60 PKL58:PKL60 PKT58:PKT60 PLB58:PLB60 PLJ58:PLJ60 PLR58:PLR60 PLZ58:PLZ60 PMH58:PMH60 PMP58:PMP60 PMX58:PMX60 PNF58:PNF60 PNN58:PNN60 PNV58:PNV60 POD58:POD60 POL58:POL60 POT58:POT60 PPB58:PPB60 PPJ58:PPJ60 PPR58:PPR60 PPZ58:PPZ60 PQH58:PQH60 PQP58:PQP60 PQX58:PQX60 PRF58:PRF60 PRN58:PRN60 PRV58:PRV60 PSD58:PSD60 PSL58:PSL60 PST58:PST60 PTB58:PTB60 PTJ58:PTJ60 PTR58:PTR60 PTZ58:PTZ60 PUH58:PUH60 PUP58:PUP60 PUX58:PUX60 PVF58:PVF60 PVN58:PVN60 PVV58:PVV60 PWD58:PWD60 PWL58:PWL60 PWT58:PWT60 PXB58:PXB60 PXJ58:PXJ60 PXR58:PXR60 PXZ58:PXZ60 PYH58:PYH60 PYP58:PYP60 PYX58:PYX60 PZF58:PZF60 PZN58:PZN60 PZV58:PZV60 QAD58:QAD60 QAL58:QAL60 QAT58:QAT60 QBB58:QBB60 QBJ58:QBJ60 QBR58:QBR60 QBZ58:QBZ60 QCH58:QCH60 QCP58:QCP60 QCX58:QCX60 QDF58:QDF60 QDN58:QDN60 QDV58:QDV60 QED58:QED60 QEL58:QEL60 QET58:QET60 QFB58:QFB60 QFJ58:QFJ60 QFR58:QFR60 QFZ58:QFZ60 QGH58:QGH60 QGP58:QGP60 QGX58:QGX60 QHF58:QHF60 QHN58:QHN60 QHV58:QHV60 QID58:QID60 QIL58:QIL60 QIT58:QIT60 QJB58:QJB60 QJJ58:QJJ60 QJR58:QJR60 QJZ58:QJZ60 QKH58:QKH60 QKP58:QKP60 QKX58:QKX60 QLF58:QLF60 QLN58:QLN60 QLV58:QLV60 QMD58:QMD60 QML58:QML60 QMT58:QMT60 QNB58:QNB60 QNJ58:QNJ60 QNR58:QNR60 QNZ58:QNZ60 QOH58:QOH60 QOP58:QOP60 QOX58:QOX60 QPF58:QPF60 QPN58:QPN60 QPV58:QPV60 QQD58:QQD60 QQL58:QQL60 QQT58:QQT60 QRB58:QRB60 QRJ58:QRJ60 QRR58:QRR60 QRZ58:QRZ60 QSH58:QSH60 QSP58:QSP60 QSX58:QSX60 QTF58:QTF60 QTN58:QTN60 QTV58:QTV60 QUD58:QUD60 QUL58:QUL60 QUT58:QUT60 QVB58:QVB60 QVJ58:QVJ60 QVR58:QVR60 QVZ58:QVZ60 QWH58:QWH60 QWP58:QWP60 QWX58:QWX60 QXF58:QXF60 QXN58:QXN60 QXV58:QXV60 QYD58:QYD60 QYL58:QYL60 QYT58:QYT60 QZB58:QZB60 QZJ58:QZJ60 QZR58:QZR60 QZZ58:QZZ60 RAH58:RAH60 RAP58:RAP60 RAX58:RAX60 RBF58:RBF60 RBN58:RBN60 RBV58:RBV60 RCD58:RCD60 RCL58:RCL60 RCT58:RCT60 RDB58:RDB60 RDJ58:RDJ60 RDR58:RDR60 RDZ58:RDZ60 REH58:REH60 REP58:REP60 REX58:REX60 RFF58:RFF60 RFN58:RFN60 RFV58:RFV60 RGD58:RGD60 RGL58:RGL60 RGT58:RGT60 RHB58:RHB60 RHJ58:RHJ60 RHR58:RHR60 RHZ58:RHZ60 RIH58:RIH60 RIP58:RIP60 RIX58:RIX60 RJF58:RJF60 RJN58:RJN60 RJV58:RJV60 RKD58:RKD60 RKL58:RKL60 RKT58:RKT60 RLB58:RLB60 RLJ58:RLJ60 RLR58:RLR60 RLZ58:RLZ60 RMH58:RMH60 RMP58:RMP60 RMX58:RMX60 RNF58:RNF60 RNN58:RNN60 RNV58:RNV60 ROD58:ROD60 ROL58:ROL60 ROT58:ROT60 RPB58:RPB60 RPJ58:RPJ60 RPR58:RPR60 RPZ58:RPZ60 RQH58:RQH60 RQP58:RQP60 RQX58:RQX60 RRF58:RRF60 RRN58:RRN60 RRV58:RRV60 RSD58:RSD60 RSL58:RSL60 RST58:RST60 RTB58:RTB60 RTJ58:RTJ60 RTR58:RTR60 RTZ58:RTZ60 RUH58:RUH60 RUP58:RUP60 RUX58:RUX60 RVF58:RVF60 RVN58:RVN60 RVV58:RVV60 RWD58:RWD60 RWL58:RWL60 RWT58:RWT60 RXB58:RXB60 RXJ58:RXJ60 RXR58:RXR60 RXZ58:RXZ60 RYH58:RYH60 RYP58:RYP60 RYX58:RYX60 RZF58:RZF60 RZN58:RZN60 RZV58:RZV60 SAD58:SAD60 SAL58:SAL60 SAT58:SAT60 SBB58:SBB60 SBJ58:SBJ60 SBR58:SBR60 SBZ58:SBZ60 SCH58:SCH60 SCP58:SCP60 SCX58:SCX60 SDF58:SDF60 SDN58:SDN60 SDV58:SDV60 SED58:SED60 SEL58:SEL60 SET58:SET60 SFB58:SFB60 SFJ58:SFJ60 SFR58:SFR60 SFZ58:SFZ60 SGH58:SGH60 SGP58:SGP60 SGX58:SGX60 SHF58:SHF60 SHN58:SHN60 SHV58:SHV60 SID58:SID60 SIL58:SIL60 SIT58:SIT60 SJB58:SJB60 SJJ58:SJJ60 SJR58:SJR60 SJZ58:SJZ60 SKH58:SKH60 SKP58:SKP60 SKX58:SKX60 SLF58:SLF60 SLN58:SLN60 SLV58:SLV60 SMD58:SMD60 SML58:SML60 SMT58:SMT60 SNB58:SNB60 SNJ58:SNJ60 SNR58:SNR60 SNZ58:SNZ60 SOH58:SOH60 SOP58:SOP60 SOX58:SOX60 SPF58:SPF60 SPN58:SPN60 SPV58:SPV60 SQD58:SQD60 SQL58:SQL60 SQT58:SQT60 SRB58:SRB60 SRJ58:SRJ60 SRR58:SRR60 SRZ58:SRZ60 SSH58:SSH60 SSP58:SSP60 SSX58:SSX60 STF58:STF60 STN58:STN60 STV58:STV60 SUD58:SUD60 SUL58:SUL60 SUT58:SUT60 SVB58:SVB60 SVJ58:SVJ60 SVR58:SVR60 SVZ58:SVZ60 SWH58:SWH60 SWP58:SWP60 SWX58:SWX60 SXF58:SXF60 SXN58:SXN60 SXV58:SXV60 SYD58:SYD60 SYL58:SYL60 SYT58:SYT60 SZB58:SZB60 SZJ58:SZJ60 SZR58:SZR60 SZZ58:SZZ60 TAH58:TAH60 TAP58:TAP60 TAX58:TAX60 TBF58:TBF60 TBN58:TBN60 TBV58:TBV60 TCD58:TCD60 TCL58:TCL60 TCT58:TCT60 TDB58:TDB60 TDJ58:TDJ60 TDR58:TDR60 TDZ58:TDZ60 TEH58:TEH60 TEP58:TEP60 TEX58:TEX60 TFF58:TFF60 TFN58:TFN60 TFV58:TFV60 TGD58:TGD60 TGL58:TGL60 TGT58:TGT60 THB58:THB60 THJ58:THJ60 THR58:THR60 THZ58:THZ60 TIH58:TIH60 TIP58:TIP60 TIX58:TIX60 TJF58:TJF60 TJN58:TJN60 TJV58:TJV60 TKD58:TKD60 TKL58:TKL60 TKT58:TKT60 TLB58:TLB60 TLJ58:TLJ60 TLR58:TLR60 TLZ58:TLZ60 TMH58:TMH60 TMP58:TMP60 TMX58:TMX60 TNF58:TNF60 TNN58:TNN60 TNV58:TNV60 TOD58:TOD60 TOL58:TOL60 TOT58:TOT60 TPB58:TPB60 TPJ58:TPJ60 TPR58:TPR60 TPZ58:TPZ60 TQH58:TQH60 TQP58:TQP60 TQX58:TQX60 TRF58:TRF60 TRN58:TRN60 TRV58:TRV60 TSD58:TSD60 TSL58:TSL60 TST58:TST60 TTB58:TTB60 TTJ58:TTJ60 TTR58:TTR60 TTZ58:TTZ60 TUH58:TUH60 TUP58:TUP60 TUX58:TUX60 TVF58:TVF60 TVN58:TVN60 TVV58:TVV60 TWD58:TWD60 TWL58:TWL60 TWT58:TWT60 TXB58:TXB60 TXJ58:TXJ60 TXR58:TXR60 TXZ58:TXZ60 TYH58:TYH60 TYP58:TYP60 TYX58:TYX60 TZF58:TZF60 TZN58:TZN60 TZV58:TZV60 UAD58:UAD60 UAL58:UAL60 UAT58:UAT60 UBB58:UBB60 UBJ58:UBJ60 UBR58:UBR60 UBZ58:UBZ60 UCH58:UCH60 UCP58:UCP60 UCX58:UCX60 UDF58:UDF60 UDN58:UDN60 UDV58:UDV60 UED58:UED60 UEL58:UEL60 UET58:UET60 UFB58:UFB60 UFJ58:UFJ60 UFR58:UFR60 UFZ58:UFZ60 UGH58:UGH60 UGP58:UGP60 UGX58:UGX60 UHF58:UHF60 UHN58:UHN60 UHV58:UHV60 UID58:UID60 UIL58:UIL60 UIT58:UIT60 UJB58:UJB60 UJJ58:UJJ60 UJR58:UJR60 UJZ58:UJZ60 UKH58:UKH60 UKP58:UKP60 UKX58:UKX60 ULF58:ULF60 ULN58:ULN60 ULV58:ULV60 UMD58:UMD60 UML58:UML60 UMT58:UMT60 UNB58:UNB60 UNJ58:UNJ60 UNR58:UNR60 UNZ58:UNZ60 UOH58:UOH60 UOP58:UOP60 UOX58:UOX60 UPF58:UPF60 UPN58:UPN60 UPV58:UPV60 UQD58:UQD60 UQL58:UQL60 UQT58:UQT60 URB58:URB60 URJ58:URJ60 URR58:URR60 URZ58:URZ60 USH58:USH60 USP58:USP60 USX58:USX60 UTF58:UTF60 UTN58:UTN60 UTV58:UTV60 UUD58:UUD60 UUL58:UUL60 UUT58:UUT60 UVB58:UVB60 UVJ58:UVJ60 UVR58:UVR60 UVZ58:UVZ60 UWH58:UWH60 UWP58:UWP60 UWX58:UWX60 UXF58:UXF60 UXN58:UXN60 UXV58:UXV60 UYD58:UYD60 UYL58:UYL60 UYT58:UYT60 UZB58:UZB60 UZJ58:UZJ60 UZR58:UZR60 UZZ58:UZZ60 VAH58:VAH60 VAP58:VAP60 VAX58:VAX60 VBF58:VBF60 VBN58:VBN60 VBV58:VBV60 VCD58:VCD60 VCL58:VCL60 VCT58:VCT60 VDB58:VDB60 VDJ58:VDJ60 VDR58:VDR60 VDZ58:VDZ60 VEH58:VEH60 VEP58:VEP60 VEX58:VEX60 VFF58:VFF60 VFN58:VFN60 VFV58:VFV60 VGD58:VGD60 VGL58:VGL60 VGT58:VGT60 VHB58:VHB60 VHJ58:VHJ60 VHR58:VHR60 VHZ58:VHZ60 VIH58:VIH60 VIP58:VIP60 VIX58:VIX60 VJF58:VJF60 VJN58:VJN60 VJV58:VJV60 VKD58:VKD60 VKL58:VKL60 VKT58:VKT60 VLB58:VLB60 VLJ58:VLJ60 VLR58:VLR60 VLZ58:VLZ60 VMH58:VMH60 VMP58:VMP60 VMX58:VMX60 VNF58:VNF60 VNN58:VNN60 VNV58:VNV60 VOD58:VOD60 VOL58:VOL60 VOT58:VOT60 VPB58:VPB60 VPJ58:VPJ60 VPR58:VPR60 VPZ58:VPZ60 VQH58:VQH60 VQP58:VQP60 VQX58:VQX60 VRF58:VRF60 VRN58:VRN60 VRV58:VRV60 VSD58:VSD60 VSL58:VSL60 VST58:VST60 VTB58:VTB60 VTJ58:VTJ60 VTR58:VTR60 VTZ58:VTZ60 VUH58:VUH60 VUP58:VUP60 VUX58:VUX60 VVF58:VVF60 VVN58:VVN60 VVV58:VVV60 VWD58:VWD60 VWL58:VWL60 VWT58:VWT60 VXB58:VXB60 VXJ58:VXJ60 VXR58:VXR60 VXZ58:VXZ60 VYH58:VYH60 VYP58:VYP60 VYX58:VYX60 VZF58:VZF60 VZN58:VZN60 VZV58:VZV60 WAD58:WAD60 WAL58:WAL60 WAT58:WAT60 WBB58:WBB60 WBJ58:WBJ60 WBR58:WBR60 WBZ58:WBZ60 WCH58:WCH60 WCP58:WCP60 WCX58:WCX60 WDF58:WDF60 WDN58:WDN60 WDV58:WDV60 WED58:WED60 WEL58:WEL60 WET58:WET60 WFB58:WFB60 WFJ58:WFJ60 WFR58:WFR60 WFZ58:WFZ60 WGH58:WGH60 WGP58:WGP60 WGX58:WGX60 WHF58:WHF60 WHN58:WHN60 WHV58:WHV60 WID58:WID60 WIL58:WIL60 WIT58:WIT60 WJB58:WJB60 WJJ58:WJJ60 WJR58:WJR60 WJZ58:WJZ60 WKH58:WKH60 WKP58:WKP60 WKX58:WKX60 WLF58:WLF60 WLN58:WLN60 WLV58:WLV60 WMD58:WMD60 WML58:WML60 WMT58:WMT60 WNB58:WNB60 WNJ58:WNJ60 WNR58:WNR60 WNZ58:WNZ60 WOH58:WOH60 WOP58:WOP60 WOX58:WOX60 WPF58:WPF60 WPN58:WPN60 WPV58:WPV60 WQD58:WQD60 WQL58:WQL60 WQT58:WQT60 WRB58:WRB60 WRJ58:WRJ60 WRR58:WRR60 WRZ58:WRZ60 WSH58:WSH60 WSP58:WSP60 WSX58:WSX60 WTF58:WTF60 WTN58:WTN60 WTV58:WTV60 WUD58:WUD60 WUL58:WUL60 WUT58:WUT60 WVB58:WVB60 WVJ58:WVJ60 WVR58:WVR60 WVZ58:WVZ60 WWH58:WWH60 WWP58:WWP60 WWX58:WWX60 WXF58:WXF60 WXN58:WXN60 WXV58:WXV60 WYD58:WYD60 WYL58:WYL60 WYT58:WYT60 WZB58:WZB60 WZJ58:WZJ60 WZR58:WZR60 WZZ58:WZZ60 XAH58:XAH60 XAP58:XAP60 XAX58:XAX60 XBF58:XBF60 XBN58:XBN60 XBV58:XBV60 XCD58:XCD60 XCL58:XCL60 XCT58:XCT60 XDB58:XDB60 XDJ58:XDJ60 XDR58:XDR60 XDZ58:XDZ60 XEH58:XEH60 XEP58:XEP60 XEX58:XEX60 B65:B66 B3:B63</xm:sqref>
+          <xm:sqref>B83:B1025 B71:B75 J61:J63 R61:R63 Z61:Z63 AH61:AH63 AP61:AP63 AX61:AX63 BF61:BF63 BN61:BN63 BV61:BV63 CD61:CD63 CL61:CL63 CT61:CT63 DB61:DB63 DJ61:DJ63 DR61:DR63 DZ61:DZ63 EH61:EH63 EP61:EP63 EX61:EX63 FF61:FF63 FN61:FN63 FV61:FV63 GD61:GD63 GL61:GL63 GT61:GT63 HB61:HB63 HJ61:HJ63 HR61:HR63 HZ61:HZ63 IH61:IH63 IP61:IP63 IX61:IX63 JF61:JF63 JN61:JN63 JV61:JV63 KD61:KD63 KL61:KL63 KT61:KT63 LB61:LB63 LJ61:LJ63 LR61:LR63 LZ61:LZ63 MH61:MH63 MP61:MP63 MX61:MX63 NF61:NF63 NN61:NN63 NV61:NV63 OD61:OD63 OL61:OL63 OT61:OT63 PB61:PB63 PJ61:PJ63 PR61:PR63 PZ61:PZ63 QH61:QH63 QP61:QP63 QX61:QX63 RF61:RF63 RN61:RN63 RV61:RV63 SD61:SD63 SL61:SL63 ST61:ST63 TB61:TB63 TJ61:TJ63 TR61:TR63 TZ61:TZ63 UH61:UH63 UP61:UP63 UX61:UX63 VF61:VF63 VN61:VN63 VV61:VV63 WD61:WD63 WL61:WL63 WT61:WT63 XB61:XB63 XJ61:XJ63 XR61:XR63 XZ61:XZ63 YH61:YH63 YP61:YP63 YX61:YX63 ZF61:ZF63 ZN61:ZN63 ZV61:ZV63 AAD61:AAD63 AAL61:AAL63 AAT61:AAT63 ABB61:ABB63 ABJ61:ABJ63 ABR61:ABR63 ABZ61:ABZ63 ACH61:ACH63 ACP61:ACP63 ACX61:ACX63 ADF61:ADF63 ADN61:ADN63 ADV61:ADV63 AED61:AED63 AEL61:AEL63 AET61:AET63 AFB61:AFB63 AFJ61:AFJ63 AFR61:AFR63 AFZ61:AFZ63 AGH61:AGH63 AGP61:AGP63 AGX61:AGX63 AHF61:AHF63 AHN61:AHN63 AHV61:AHV63 AID61:AID63 AIL61:AIL63 AIT61:AIT63 AJB61:AJB63 AJJ61:AJJ63 AJR61:AJR63 AJZ61:AJZ63 AKH61:AKH63 AKP61:AKP63 AKX61:AKX63 ALF61:ALF63 ALN61:ALN63 ALV61:ALV63 AMD61:AMD63 AML61:AML63 AMT61:AMT63 ANB61:ANB63 ANJ61:ANJ63 ANR61:ANR63 ANZ61:ANZ63 AOH61:AOH63 AOP61:AOP63 AOX61:AOX63 APF61:APF63 APN61:APN63 APV61:APV63 AQD61:AQD63 AQL61:AQL63 AQT61:AQT63 ARB61:ARB63 ARJ61:ARJ63 ARR61:ARR63 ARZ61:ARZ63 ASH61:ASH63 ASP61:ASP63 ASX61:ASX63 ATF61:ATF63 ATN61:ATN63 ATV61:ATV63 AUD61:AUD63 AUL61:AUL63 AUT61:AUT63 AVB61:AVB63 AVJ61:AVJ63 AVR61:AVR63 AVZ61:AVZ63 AWH61:AWH63 AWP61:AWP63 AWX61:AWX63 AXF61:AXF63 AXN61:AXN63 AXV61:AXV63 AYD61:AYD63 AYL61:AYL63 AYT61:AYT63 AZB61:AZB63 AZJ61:AZJ63 AZR61:AZR63 AZZ61:AZZ63 BAH61:BAH63 BAP61:BAP63 BAX61:BAX63 BBF61:BBF63 BBN61:BBN63 BBV61:BBV63 BCD61:BCD63 BCL61:BCL63 BCT61:BCT63 BDB61:BDB63 BDJ61:BDJ63 BDR61:BDR63 BDZ61:BDZ63 BEH61:BEH63 BEP61:BEP63 BEX61:BEX63 BFF61:BFF63 BFN61:BFN63 BFV61:BFV63 BGD61:BGD63 BGL61:BGL63 BGT61:BGT63 BHB61:BHB63 BHJ61:BHJ63 BHR61:BHR63 BHZ61:BHZ63 BIH61:BIH63 BIP61:BIP63 BIX61:BIX63 BJF61:BJF63 BJN61:BJN63 BJV61:BJV63 BKD61:BKD63 BKL61:BKL63 BKT61:BKT63 BLB61:BLB63 BLJ61:BLJ63 BLR61:BLR63 BLZ61:BLZ63 BMH61:BMH63 BMP61:BMP63 BMX61:BMX63 BNF61:BNF63 BNN61:BNN63 BNV61:BNV63 BOD61:BOD63 BOL61:BOL63 BOT61:BOT63 BPB61:BPB63 BPJ61:BPJ63 BPR61:BPR63 BPZ61:BPZ63 BQH61:BQH63 BQP61:BQP63 BQX61:BQX63 BRF61:BRF63 BRN61:BRN63 BRV61:BRV63 BSD61:BSD63 BSL61:BSL63 BST61:BST63 BTB61:BTB63 BTJ61:BTJ63 BTR61:BTR63 BTZ61:BTZ63 BUH61:BUH63 BUP61:BUP63 BUX61:BUX63 BVF61:BVF63 BVN61:BVN63 BVV61:BVV63 BWD61:BWD63 BWL61:BWL63 BWT61:BWT63 BXB61:BXB63 BXJ61:BXJ63 BXR61:BXR63 BXZ61:BXZ63 BYH61:BYH63 BYP61:BYP63 BYX61:BYX63 BZF61:BZF63 BZN61:BZN63 BZV61:BZV63 CAD61:CAD63 CAL61:CAL63 CAT61:CAT63 CBB61:CBB63 CBJ61:CBJ63 CBR61:CBR63 CBZ61:CBZ63 CCH61:CCH63 CCP61:CCP63 CCX61:CCX63 CDF61:CDF63 CDN61:CDN63 CDV61:CDV63 CED61:CED63 CEL61:CEL63 CET61:CET63 CFB61:CFB63 CFJ61:CFJ63 CFR61:CFR63 CFZ61:CFZ63 CGH61:CGH63 CGP61:CGP63 CGX61:CGX63 CHF61:CHF63 CHN61:CHN63 CHV61:CHV63 CID61:CID63 CIL61:CIL63 CIT61:CIT63 CJB61:CJB63 CJJ61:CJJ63 CJR61:CJR63 CJZ61:CJZ63 CKH61:CKH63 CKP61:CKP63 CKX61:CKX63 CLF61:CLF63 CLN61:CLN63 CLV61:CLV63 CMD61:CMD63 CML61:CML63 CMT61:CMT63 CNB61:CNB63 CNJ61:CNJ63 CNR61:CNR63 CNZ61:CNZ63 COH61:COH63 COP61:COP63 COX61:COX63 CPF61:CPF63 CPN61:CPN63 CPV61:CPV63 CQD61:CQD63 CQL61:CQL63 CQT61:CQT63 CRB61:CRB63 CRJ61:CRJ63 CRR61:CRR63 CRZ61:CRZ63 CSH61:CSH63 CSP61:CSP63 CSX61:CSX63 CTF61:CTF63 CTN61:CTN63 CTV61:CTV63 CUD61:CUD63 CUL61:CUL63 CUT61:CUT63 CVB61:CVB63 CVJ61:CVJ63 CVR61:CVR63 CVZ61:CVZ63 CWH61:CWH63 CWP61:CWP63 CWX61:CWX63 CXF61:CXF63 CXN61:CXN63 CXV61:CXV63 CYD61:CYD63 CYL61:CYL63 CYT61:CYT63 CZB61:CZB63 CZJ61:CZJ63 CZR61:CZR63 CZZ61:CZZ63 DAH61:DAH63 DAP61:DAP63 DAX61:DAX63 DBF61:DBF63 DBN61:DBN63 DBV61:DBV63 DCD61:DCD63 DCL61:DCL63 DCT61:DCT63 DDB61:DDB63 DDJ61:DDJ63 DDR61:DDR63 DDZ61:DDZ63 DEH61:DEH63 DEP61:DEP63 DEX61:DEX63 DFF61:DFF63 DFN61:DFN63 DFV61:DFV63 DGD61:DGD63 DGL61:DGL63 DGT61:DGT63 DHB61:DHB63 DHJ61:DHJ63 DHR61:DHR63 DHZ61:DHZ63 DIH61:DIH63 DIP61:DIP63 DIX61:DIX63 DJF61:DJF63 DJN61:DJN63 DJV61:DJV63 DKD61:DKD63 DKL61:DKL63 DKT61:DKT63 DLB61:DLB63 DLJ61:DLJ63 DLR61:DLR63 DLZ61:DLZ63 DMH61:DMH63 DMP61:DMP63 DMX61:DMX63 DNF61:DNF63 DNN61:DNN63 DNV61:DNV63 DOD61:DOD63 DOL61:DOL63 DOT61:DOT63 DPB61:DPB63 DPJ61:DPJ63 DPR61:DPR63 DPZ61:DPZ63 DQH61:DQH63 DQP61:DQP63 DQX61:DQX63 DRF61:DRF63 DRN61:DRN63 DRV61:DRV63 DSD61:DSD63 DSL61:DSL63 DST61:DST63 DTB61:DTB63 DTJ61:DTJ63 DTR61:DTR63 DTZ61:DTZ63 DUH61:DUH63 DUP61:DUP63 DUX61:DUX63 DVF61:DVF63 DVN61:DVN63 DVV61:DVV63 DWD61:DWD63 DWL61:DWL63 DWT61:DWT63 DXB61:DXB63 DXJ61:DXJ63 DXR61:DXR63 DXZ61:DXZ63 DYH61:DYH63 DYP61:DYP63 DYX61:DYX63 DZF61:DZF63 DZN61:DZN63 DZV61:DZV63 EAD61:EAD63 EAL61:EAL63 EAT61:EAT63 EBB61:EBB63 EBJ61:EBJ63 EBR61:EBR63 EBZ61:EBZ63 ECH61:ECH63 ECP61:ECP63 ECX61:ECX63 EDF61:EDF63 EDN61:EDN63 EDV61:EDV63 EED61:EED63 EEL61:EEL63 EET61:EET63 EFB61:EFB63 EFJ61:EFJ63 EFR61:EFR63 EFZ61:EFZ63 EGH61:EGH63 EGP61:EGP63 EGX61:EGX63 EHF61:EHF63 EHN61:EHN63 EHV61:EHV63 EID61:EID63 EIL61:EIL63 EIT61:EIT63 EJB61:EJB63 EJJ61:EJJ63 EJR61:EJR63 EJZ61:EJZ63 EKH61:EKH63 EKP61:EKP63 EKX61:EKX63 ELF61:ELF63 ELN61:ELN63 ELV61:ELV63 EMD61:EMD63 EML61:EML63 EMT61:EMT63 ENB61:ENB63 ENJ61:ENJ63 ENR61:ENR63 ENZ61:ENZ63 EOH61:EOH63 EOP61:EOP63 EOX61:EOX63 EPF61:EPF63 EPN61:EPN63 EPV61:EPV63 EQD61:EQD63 EQL61:EQL63 EQT61:EQT63 ERB61:ERB63 ERJ61:ERJ63 ERR61:ERR63 ERZ61:ERZ63 ESH61:ESH63 ESP61:ESP63 ESX61:ESX63 ETF61:ETF63 ETN61:ETN63 ETV61:ETV63 EUD61:EUD63 EUL61:EUL63 EUT61:EUT63 EVB61:EVB63 EVJ61:EVJ63 EVR61:EVR63 EVZ61:EVZ63 EWH61:EWH63 EWP61:EWP63 EWX61:EWX63 EXF61:EXF63 EXN61:EXN63 EXV61:EXV63 EYD61:EYD63 EYL61:EYL63 EYT61:EYT63 EZB61:EZB63 EZJ61:EZJ63 EZR61:EZR63 EZZ61:EZZ63 FAH61:FAH63 FAP61:FAP63 FAX61:FAX63 FBF61:FBF63 FBN61:FBN63 FBV61:FBV63 FCD61:FCD63 FCL61:FCL63 FCT61:FCT63 FDB61:FDB63 FDJ61:FDJ63 FDR61:FDR63 FDZ61:FDZ63 FEH61:FEH63 FEP61:FEP63 FEX61:FEX63 FFF61:FFF63 FFN61:FFN63 FFV61:FFV63 FGD61:FGD63 FGL61:FGL63 FGT61:FGT63 FHB61:FHB63 FHJ61:FHJ63 FHR61:FHR63 FHZ61:FHZ63 FIH61:FIH63 FIP61:FIP63 FIX61:FIX63 FJF61:FJF63 FJN61:FJN63 FJV61:FJV63 FKD61:FKD63 FKL61:FKL63 FKT61:FKT63 FLB61:FLB63 FLJ61:FLJ63 FLR61:FLR63 FLZ61:FLZ63 FMH61:FMH63 FMP61:FMP63 FMX61:FMX63 FNF61:FNF63 FNN61:FNN63 FNV61:FNV63 FOD61:FOD63 FOL61:FOL63 FOT61:FOT63 FPB61:FPB63 FPJ61:FPJ63 FPR61:FPR63 FPZ61:FPZ63 FQH61:FQH63 FQP61:FQP63 FQX61:FQX63 FRF61:FRF63 FRN61:FRN63 FRV61:FRV63 FSD61:FSD63 FSL61:FSL63 FST61:FST63 FTB61:FTB63 FTJ61:FTJ63 FTR61:FTR63 FTZ61:FTZ63 FUH61:FUH63 FUP61:FUP63 FUX61:FUX63 FVF61:FVF63 FVN61:FVN63 FVV61:FVV63 FWD61:FWD63 FWL61:FWL63 FWT61:FWT63 FXB61:FXB63 FXJ61:FXJ63 FXR61:FXR63 FXZ61:FXZ63 FYH61:FYH63 FYP61:FYP63 FYX61:FYX63 FZF61:FZF63 FZN61:FZN63 FZV61:FZV63 GAD61:GAD63 GAL61:GAL63 GAT61:GAT63 GBB61:GBB63 GBJ61:GBJ63 GBR61:GBR63 GBZ61:GBZ63 GCH61:GCH63 GCP61:GCP63 GCX61:GCX63 GDF61:GDF63 GDN61:GDN63 GDV61:GDV63 GED61:GED63 GEL61:GEL63 GET61:GET63 GFB61:GFB63 GFJ61:GFJ63 GFR61:GFR63 GFZ61:GFZ63 GGH61:GGH63 GGP61:GGP63 GGX61:GGX63 GHF61:GHF63 GHN61:GHN63 GHV61:GHV63 GID61:GID63 GIL61:GIL63 GIT61:GIT63 GJB61:GJB63 GJJ61:GJJ63 GJR61:GJR63 GJZ61:GJZ63 GKH61:GKH63 GKP61:GKP63 GKX61:GKX63 GLF61:GLF63 GLN61:GLN63 GLV61:GLV63 GMD61:GMD63 GML61:GML63 GMT61:GMT63 GNB61:GNB63 GNJ61:GNJ63 GNR61:GNR63 GNZ61:GNZ63 GOH61:GOH63 GOP61:GOP63 GOX61:GOX63 GPF61:GPF63 GPN61:GPN63 GPV61:GPV63 GQD61:GQD63 GQL61:GQL63 GQT61:GQT63 GRB61:GRB63 GRJ61:GRJ63 GRR61:GRR63 GRZ61:GRZ63 GSH61:GSH63 GSP61:GSP63 GSX61:GSX63 GTF61:GTF63 GTN61:GTN63 GTV61:GTV63 GUD61:GUD63 GUL61:GUL63 GUT61:GUT63 GVB61:GVB63 GVJ61:GVJ63 GVR61:GVR63 GVZ61:GVZ63 GWH61:GWH63 GWP61:GWP63 GWX61:GWX63 GXF61:GXF63 GXN61:GXN63 GXV61:GXV63 GYD61:GYD63 GYL61:GYL63 GYT61:GYT63 GZB61:GZB63 GZJ61:GZJ63 GZR61:GZR63 GZZ61:GZZ63 HAH61:HAH63 HAP61:HAP63 HAX61:HAX63 HBF61:HBF63 HBN61:HBN63 HBV61:HBV63 HCD61:HCD63 HCL61:HCL63 HCT61:HCT63 HDB61:HDB63 HDJ61:HDJ63 HDR61:HDR63 HDZ61:HDZ63 HEH61:HEH63 HEP61:HEP63 HEX61:HEX63 HFF61:HFF63 HFN61:HFN63 HFV61:HFV63 HGD61:HGD63 HGL61:HGL63 HGT61:HGT63 HHB61:HHB63 HHJ61:HHJ63 HHR61:HHR63 HHZ61:HHZ63 HIH61:HIH63 HIP61:HIP63 HIX61:HIX63 HJF61:HJF63 HJN61:HJN63 HJV61:HJV63 HKD61:HKD63 HKL61:HKL63 HKT61:HKT63 HLB61:HLB63 HLJ61:HLJ63 HLR61:HLR63 HLZ61:HLZ63 HMH61:HMH63 HMP61:HMP63 HMX61:HMX63 HNF61:HNF63 HNN61:HNN63 HNV61:HNV63 HOD61:HOD63 HOL61:HOL63 HOT61:HOT63 HPB61:HPB63 HPJ61:HPJ63 HPR61:HPR63 HPZ61:HPZ63 HQH61:HQH63 HQP61:HQP63 HQX61:HQX63 HRF61:HRF63 HRN61:HRN63 HRV61:HRV63 HSD61:HSD63 HSL61:HSL63 HST61:HST63 HTB61:HTB63 HTJ61:HTJ63 HTR61:HTR63 HTZ61:HTZ63 HUH61:HUH63 HUP61:HUP63 HUX61:HUX63 HVF61:HVF63 HVN61:HVN63 HVV61:HVV63 HWD61:HWD63 HWL61:HWL63 HWT61:HWT63 HXB61:HXB63 HXJ61:HXJ63 HXR61:HXR63 HXZ61:HXZ63 HYH61:HYH63 HYP61:HYP63 HYX61:HYX63 HZF61:HZF63 HZN61:HZN63 HZV61:HZV63 IAD61:IAD63 IAL61:IAL63 IAT61:IAT63 IBB61:IBB63 IBJ61:IBJ63 IBR61:IBR63 IBZ61:IBZ63 ICH61:ICH63 ICP61:ICP63 ICX61:ICX63 IDF61:IDF63 IDN61:IDN63 IDV61:IDV63 IED61:IED63 IEL61:IEL63 IET61:IET63 IFB61:IFB63 IFJ61:IFJ63 IFR61:IFR63 IFZ61:IFZ63 IGH61:IGH63 IGP61:IGP63 IGX61:IGX63 IHF61:IHF63 IHN61:IHN63 IHV61:IHV63 IID61:IID63 IIL61:IIL63 IIT61:IIT63 IJB61:IJB63 IJJ61:IJJ63 IJR61:IJR63 IJZ61:IJZ63 IKH61:IKH63 IKP61:IKP63 IKX61:IKX63 ILF61:ILF63 ILN61:ILN63 ILV61:ILV63 IMD61:IMD63 IML61:IML63 IMT61:IMT63 INB61:INB63 INJ61:INJ63 INR61:INR63 INZ61:INZ63 IOH61:IOH63 IOP61:IOP63 IOX61:IOX63 IPF61:IPF63 IPN61:IPN63 IPV61:IPV63 IQD61:IQD63 IQL61:IQL63 IQT61:IQT63 IRB61:IRB63 IRJ61:IRJ63 IRR61:IRR63 IRZ61:IRZ63 ISH61:ISH63 ISP61:ISP63 ISX61:ISX63 ITF61:ITF63 ITN61:ITN63 ITV61:ITV63 IUD61:IUD63 IUL61:IUL63 IUT61:IUT63 IVB61:IVB63 IVJ61:IVJ63 IVR61:IVR63 IVZ61:IVZ63 IWH61:IWH63 IWP61:IWP63 IWX61:IWX63 IXF61:IXF63 IXN61:IXN63 IXV61:IXV63 IYD61:IYD63 IYL61:IYL63 IYT61:IYT63 IZB61:IZB63 IZJ61:IZJ63 IZR61:IZR63 IZZ61:IZZ63 JAH61:JAH63 JAP61:JAP63 JAX61:JAX63 JBF61:JBF63 JBN61:JBN63 JBV61:JBV63 JCD61:JCD63 JCL61:JCL63 JCT61:JCT63 JDB61:JDB63 JDJ61:JDJ63 JDR61:JDR63 JDZ61:JDZ63 JEH61:JEH63 JEP61:JEP63 JEX61:JEX63 JFF61:JFF63 JFN61:JFN63 JFV61:JFV63 JGD61:JGD63 JGL61:JGL63 JGT61:JGT63 JHB61:JHB63 JHJ61:JHJ63 JHR61:JHR63 JHZ61:JHZ63 JIH61:JIH63 JIP61:JIP63 JIX61:JIX63 JJF61:JJF63 JJN61:JJN63 JJV61:JJV63 JKD61:JKD63 JKL61:JKL63 JKT61:JKT63 JLB61:JLB63 JLJ61:JLJ63 JLR61:JLR63 JLZ61:JLZ63 JMH61:JMH63 JMP61:JMP63 JMX61:JMX63 JNF61:JNF63 JNN61:JNN63 JNV61:JNV63 JOD61:JOD63 JOL61:JOL63 JOT61:JOT63 JPB61:JPB63 JPJ61:JPJ63 JPR61:JPR63 JPZ61:JPZ63 JQH61:JQH63 JQP61:JQP63 JQX61:JQX63 JRF61:JRF63 JRN61:JRN63 JRV61:JRV63 JSD61:JSD63 JSL61:JSL63 JST61:JST63 JTB61:JTB63 JTJ61:JTJ63 JTR61:JTR63 JTZ61:JTZ63 JUH61:JUH63 JUP61:JUP63 JUX61:JUX63 JVF61:JVF63 JVN61:JVN63 JVV61:JVV63 JWD61:JWD63 JWL61:JWL63 JWT61:JWT63 JXB61:JXB63 JXJ61:JXJ63 JXR61:JXR63 JXZ61:JXZ63 JYH61:JYH63 JYP61:JYP63 JYX61:JYX63 JZF61:JZF63 JZN61:JZN63 JZV61:JZV63 KAD61:KAD63 KAL61:KAL63 KAT61:KAT63 KBB61:KBB63 KBJ61:KBJ63 KBR61:KBR63 KBZ61:KBZ63 KCH61:KCH63 KCP61:KCP63 KCX61:KCX63 KDF61:KDF63 KDN61:KDN63 KDV61:KDV63 KED61:KED63 KEL61:KEL63 KET61:KET63 KFB61:KFB63 KFJ61:KFJ63 KFR61:KFR63 KFZ61:KFZ63 KGH61:KGH63 KGP61:KGP63 KGX61:KGX63 KHF61:KHF63 KHN61:KHN63 KHV61:KHV63 KID61:KID63 KIL61:KIL63 KIT61:KIT63 KJB61:KJB63 KJJ61:KJJ63 KJR61:KJR63 KJZ61:KJZ63 KKH61:KKH63 KKP61:KKP63 KKX61:KKX63 KLF61:KLF63 KLN61:KLN63 KLV61:KLV63 KMD61:KMD63 KML61:KML63 KMT61:KMT63 KNB61:KNB63 KNJ61:KNJ63 KNR61:KNR63 KNZ61:KNZ63 KOH61:KOH63 KOP61:KOP63 KOX61:KOX63 KPF61:KPF63 KPN61:KPN63 KPV61:KPV63 KQD61:KQD63 KQL61:KQL63 KQT61:KQT63 KRB61:KRB63 KRJ61:KRJ63 KRR61:KRR63 KRZ61:KRZ63 KSH61:KSH63 KSP61:KSP63 KSX61:KSX63 KTF61:KTF63 KTN61:KTN63 KTV61:KTV63 KUD61:KUD63 KUL61:KUL63 KUT61:KUT63 KVB61:KVB63 KVJ61:KVJ63 KVR61:KVR63 KVZ61:KVZ63 KWH61:KWH63 KWP61:KWP63 KWX61:KWX63 KXF61:KXF63 KXN61:KXN63 KXV61:KXV63 KYD61:KYD63 KYL61:KYL63 KYT61:KYT63 KZB61:KZB63 KZJ61:KZJ63 KZR61:KZR63 KZZ61:KZZ63 LAH61:LAH63 LAP61:LAP63 LAX61:LAX63 LBF61:LBF63 LBN61:LBN63 LBV61:LBV63 LCD61:LCD63 LCL61:LCL63 LCT61:LCT63 LDB61:LDB63 LDJ61:LDJ63 LDR61:LDR63 LDZ61:LDZ63 LEH61:LEH63 LEP61:LEP63 LEX61:LEX63 LFF61:LFF63 LFN61:LFN63 LFV61:LFV63 LGD61:LGD63 LGL61:LGL63 LGT61:LGT63 LHB61:LHB63 LHJ61:LHJ63 LHR61:LHR63 LHZ61:LHZ63 LIH61:LIH63 LIP61:LIP63 LIX61:LIX63 LJF61:LJF63 LJN61:LJN63 LJV61:LJV63 LKD61:LKD63 LKL61:LKL63 LKT61:LKT63 LLB61:LLB63 LLJ61:LLJ63 LLR61:LLR63 LLZ61:LLZ63 LMH61:LMH63 LMP61:LMP63 LMX61:LMX63 LNF61:LNF63 LNN61:LNN63 LNV61:LNV63 LOD61:LOD63 LOL61:LOL63 LOT61:LOT63 LPB61:LPB63 LPJ61:LPJ63 LPR61:LPR63 LPZ61:LPZ63 LQH61:LQH63 LQP61:LQP63 LQX61:LQX63 LRF61:LRF63 LRN61:LRN63 LRV61:LRV63 LSD61:LSD63 LSL61:LSL63 LST61:LST63 LTB61:LTB63 LTJ61:LTJ63 LTR61:LTR63 LTZ61:LTZ63 LUH61:LUH63 LUP61:LUP63 LUX61:LUX63 LVF61:LVF63 LVN61:LVN63 LVV61:LVV63 LWD61:LWD63 LWL61:LWL63 LWT61:LWT63 LXB61:LXB63 LXJ61:LXJ63 LXR61:LXR63 LXZ61:LXZ63 LYH61:LYH63 LYP61:LYP63 LYX61:LYX63 LZF61:LZF63 LZN61:LZN63 LZV61:LZV63 MAD61:MAD63 MAL61:MAL63 MAT61:MAT63 MBB61:MBB63 MBJ61:MBJ63 MBR61:MBR63 MBZ61:MBZ63 MCH61:MCH63 MCP61:MCP63 MCX61:MCX63 MDF61:MDF63 MDN61:MDN63 MDV61:MDV63 MED61:MED63 MEL61:MEL63 MET61:MET63 MFB61:MFB63 MFJ61:MFJ63 MFR61:MFR63 MFZ61:MFZ63 MGH61:MGH63 MGP61:MGP63 MGX61:MGX63 MHF61:MHF63 MHN61:MHN63 MHV61:MHV63 MID61:MID63 MIL61:MIL63 MIT61:MIT63 MJB61:MJB63 MJJ61:MJJ63 MJR61:MJR63 MJZ61:MJZ63 MKH61:MKH63 MKP61:MKP63 MKX61:MKX63 MLF61:MLF63 MLN61:MLN63 MLV61:MLV63 MMD61:MMD63 MML61:MML63 MMT61:MMT63 MNB61:MNB63 MNJ61:MNJ63 MNR61:MNR63 MNZ61:MNZ63 MOH61:MOH63 MOP61:MOP63 MOX61:MOX63 MPF61:MPF63 MPN61:MPN63 MPV61:MPV63 MQD61:MQD63 MQL61:MQL63 MQT61:MQT63 MRB61:MRB63 MRJ61:MRJ63 MRR61:MRR63 MRZ61:MRZ63 MSH61:MSH63 MSP61:MSP63 MSX61:MSX63 MTF61:MTF63 MTN61:MTN63 MTV61:MTV63 MUD61:MUD63 MUL61:MUL63 MUT61:MUT63 MVB61:MVB63 MVJ61:MVJ63 MVR61:MVR63 MVZ61:MVZ63 MWH61:MWH63 MWP61:MWP63 MWX61:MWX63 MXF61:MXF63 MXN61:MXN63 MXV61:MXV63 MYD61:MYD63 MYL61:MYL63 MYT61:MYT63 MZB61:MZB63 MZJ61:MZJ63 MZR61:MZR63 MZZ61:MZZ63 NAH61:NAH63 NAP61:NAP63 NAX61:NAX63 NBF61:NBF63 NBN61:NBN63 NBV61:NBV63 NCD61:NCD63 NCL61:NCL63 NCT61:NCT63 NDB61:NDB63 NDJ61:NDJ63 NDR61:NDR63 NDZ61:NDZ63 NEH61:NEH63 NEP61:NEP63 NEX61:NEX63 NFF61:NFF63 NFN61:NFN63 NFV61:NFV63 NGD61:NGD63 NGL61:NGL63 NGT61:NGT63 NHB61:NHB63 NHJ61:NHJ63 NHR61:NHR63 NHZ61:NHZ63 NIH61:NIH63 NIP61:NIP63 NIX61:NIX63 NJF61:NJF63 NJN61:NJN63 NJV61:NJV63 NKD61:NKD63 NKL61:NKL63 NKT61:NKT63 NLB61:NLB63 NLJ61:NLJ63 NLR61:NLR63 NLZ61:NLZ63 NMH61:NMH63 NMP61:NMP63 NMX61:NMX63 NNF61:NNF63 NNN61:NNN63 NNV61:NNV63 NOD61:NOD63 NOL61:NOL63 NOT61:NOT63 NPB61:NPB63 NPJ61:NPJ63 NPR61:NPR63 NPZ61:NPZ63 NQH61:NQH63 NQP61:NQP63 NQX61:NQX63 NRF61:NRF63 NRN61:NRN63 NRV61:NRV63 NSD61:NSD63 NSL61:NSL63 NST61:NST63 NTB61:NTB63 NTJ61:NTJ63 NTR61:NTR63 NTZ61:NTZ63 NUH61:NUH63 NUP61:NUP63 NUX61:NUX63 NVF61:NVF63 NVN61:NVN63 NVV61:NVV63 NWD61:NWD63 NWL61:NWL63 NWT61:NWT63 NXB61:NXB63 NXJ61:NXJ63 NXR61:NXR63 NXZ61:NXZ63 NYH61:NYH63 NYP61:NYP63 NYX61:NYX63 NZF61:NZF63 NZN61:NZN63 NZV61:NZV63 OAD61:OAD63 OAL61:OAL63 OAT61:OAT63 OBB61:OBB63 OBJ61:OBJ63 OBR61:OBR63 OBZ61:OBZ63 OCH61:OCH63 OCP61:OCP63 OCX61:OCX63 ODF61:ODF63 ODN61:ODN63 ODV61:ODV63 OED61:OED63 OEL61:OEL63 OET61:OET63 OFB61:OFB63 OFJ61:OFJ63 OFR61:OFR63 OFZ61:OFZ63 OGH61:OGH63 OGP61:OGP63 OGX61:OGX63 OHF61:OHF63 OHN61:OHN63 OHV61:OHV63 OID61:OID63 OIL61:OIL63 OIT61:OIT63 OJB61:OJB63 OJJ61:OJJ63 OJR61:OJR63 OJZ61:OJZ63 OKH61:OKH63 OKP61:OKP63 OKX61:OKX63 OLF61:OLF63 OLN61:OLN63 OLV61:OLV63 OMD61:OMD63 OML61:OML63 OMT61:OMT63 ONB61:ONB63 ONJ61:ONJ63 ONR61:ONR63 ONZ61:ONZ63 OOH61:OOH63 OOP61:OOP63 OOX61:OOX63 OPF61:OPF63 OPN61:OPN63 OPV61:OPV63 OQD61:OQD63 OQL61:OQL63 OQT61:OQT63 ORB61:ORB63 ORJ61:ORJ63 ORR61:ORR63 ORZ61:ORZ63 OSH61:OSH63 OSP61:OSP63 OSX61:OSX63 OTF61:OTF63 OTN61:OTN63 OTV61:OTV63 OUD61:OUD63 OUL61:OUL63 OUT61:OUT63 OVB61:OVB63 OVJ61:OVJ63 OVR61:OVR63 OVZ61:OVZ63 OWH61:OWH63 OWP61:OWP63 OWX61:OWX63 OXF61:OXF63 OXN61:OXN63 OXV61:OXV63 OYD61:OYD63 OYL61:OYL63 OYT61:OYT63 OZB61:OZB63 OZJ61:OZJ63 OZR61:OZR63 OZZ61:OZZ63 PAH61:PAH63 PAP61:PAP63 PAX61:PAX63 PBF61:PBF63 PBN61:PBN63 PBV61:PBV63 PCD61:PCD63 PCL61:PCL63 PCT61:PCT63 PDB61:PDB63 PDJ61:PDJ63 PDR61:PDR63 PDZ61:PDZ63 PEH61:PEH63 PEP61:PEP63 PEX61:PEX63 PFF61:PFF63 PFN61:PFN63 PFV61:PFV63 PGD61:PGD63 PGL61:PGL63 PGT61:PGT63 PHB61:PHB63 PHJ61:PHJ63 PHR61:PHR63 PHZ61:PHZ63 PIH61:PIH63 PIP61:PIP63 PIX61:PIX63 PJF61:PJF63 PJN61:PJN63 PJV61:PJV63 PKD61:PKD63 PKL61:PKL63 PKT61:PKT63 PLB61:PLB63 PLJ61:PLJ63 PLR61:PLR63 PLZ61:PLZ63 PMH61:PMH63 PMP61:PMP63 PMX61:PMX63 PNF61:PNF63 PNN61:PNN63 PNV61:PNV63 POD61:POD63 POL61:POL63 POT61:POT63 PPB61:PPB63 PPJ61:PPJ63 PPR61:PPR63 PPZ61:PPZ63 PQH61:PQH63 PQP61:PQP63 PQX61:PQX63 PRF61:PRF63 PRN61:PRN63 PRV61:PRV63 PSD61:PSD63 PSL61:PSL63 PST61:PST63 PTB61:PTB63 PTJ61:PTJ63 PTR61:PTR63 PTZ61:PTZ63 PUH61:PUH63 PUP61:PUP63 PUX61:PUX63 PVF61:PVF63 PVN61:PVN63 PVV61:PVV63 PWD61:PWD63 PWL61:PWL63 PWT61:PWT63 PXB61:PXB63 PXJ61:PXJ63 PXR61:PXR63 PXZ61:PXZ63 PYH61:PYH63 PYP61:PYP63 PYX61:PYX63 PZF61:PZF63 PZN61:PZN63 PZV61:PZV63 QAD61:QAD63 QAL61:QAL63 QAT61:QAT63 QBB61:QBB63 QBJ61:QBJ63 QBR61:QBR63 QBZ61:QBZ63 QCH61:QCH63 QCP61:QCP63 QCX61:QCX63 QDF61:QDF63 QDN61:QDN63 QDV61:QDV63 QED61:QED63 QEL61:QEL63 QET61:QET63 QFB61:QFB63 QFJ61:QFJ63 QFR61:QFR63 QFZ61:QFZ63 QGH61:QGH63 QGP61:QGP63 QGX61:QGX63 QHF61:QHF63 QHN61:QHN63 QHV61:QHV63 QID61:QID63 QIL61:QIL63 QIT61:QIT63 QJB61:QJB63 QJJ61:QJJ63 QJR61:QJR63 QJZ61:QJZ63 QKH61:QKH63 QKP61:QKP63 QKX61:QKX63 QLF61:QLF63 QLN61:QLN63 QLV61:QLV63 QMD61:QMD63 QML61:QML63 QMT61:QMT63 QNB61:QNB63 QNJ61:QNJ63 QNR61:QNR63 QNZ61:QNZ63 QOH61:QOH63 QOP61:QOP63 QOX61:QOX63 QPF61:QPF63 QPN61:QPN63 QPV61:QPV63 QQD61:QQD63 QQL61:QQL63 QQT61:QQT63 QRB61:QRB63 QRJ61:QRJ63 QRR61:QRR63 QRZ61:QRZ63 QSH61:QSH63 QSP61:QSP63 QSX61:QSX63 QTF61:QTF63 QTN61:QTN63 QTV61:QTV63 QUD61:QUD63 QUL61:QUL63 QUT61:QUT63 QVB61:QVB63 QVJ61:QVJ63 QVR61:QVR63 QVZ61:QVZ63 QWH61:QWH63 QWP61:QWP63 QWX61:QWX63 QXF61:QXF63 QXN61:QXN63 QXV61:QXV63 QYD61:QYD63 QYL61:QYL63 QYT61:QYT63 QZB61:QZB63 QZJ61:QZJ63 QZR61:QZR63 QZZ61:QZZ63 RAH61:RAH63 RAP61:RAP63 RAX61:RAX63 RBF61:RBF63 RBN61:RBN63 RBV61:RBV63 RCD61:RCD63 RCL61:RCL63 RCT61:RCT63 RDB61:RDB63 RDJ61:RDJ63 RDR61:RDR63 RDZ61:RDZ63 REH61:REH63 REP61:REP63 REX61:REX63 RFF61:RFF63 RFN61:RFN63 RFV61:RFV63 RGD61:RGD63 RGL61:RGL63 RGT61:RGT63 RHB61:RHB63 RHJ61:RHJ63 RHR61:RHR63 RHZ61:RHZ63 RIH61:RIH63 RIP61:RIP63 RIX61:RIX63 RJF61:RJF63 RJN61:RJN63 RJV61:RJV63 RKD61:RKD63 RKL61:RKL63 RKT61:RKT63 RLB61:RLB63 RLJ61:RLJ63 RLR61:RLR63 RLZ61:RLZ63 RMH61:RMH63 RMP61:RMP63 RMX61:RMX63 RNF61:RNF63 RNN61:RNN63 RNV61:RNV63 ROD61:ROD63 ROL61:ROL63 ROT61:ROT63 RPB61:RPB63 RPJ61:RPJ63 RPR61:RPR63 RPZ61:RPZ63 RQH61:RQH63 RQP61:RQP63 RQX61:RQX63 RRF61:RRF63 RRN61:RRN63 RRV61:RRV63 RSD61:RSD63 RSL61:RSL63 RST61:RST63 RTB61:RTB63 RTJ61:RTJ63 RTR61:RTR63 RTZ61:RTZ63 RUH61:RUH63 RUP61:RUP63 RUX61:RUX63 RVF61:RVF63 RVN61:RVN63 RVV61:RVV63 RWD61:RWD63 RWL61:RWL63 RWT61:RWT63 RXB61:RXB63 RXJ61:RXJ63 RXR61:RXR63 RXZ61:RXZ63 RYH61:RYH63 RYP61:RYP63 RYX61:RYX63 RZF61:RZF63 RZN61:RZN63 RZV61:RZV63 SAD61:SAD63 SAL61:SAL63 SAT61:SAT63 SBB61:SBB63 SBJ61:SBJ63 SBR61:SBR63 SBZ61:SBZ63 SCH61:SCH63 SCP61:SCP63 SCX61:SCX63 SDF61:SDF63 SDN61:SDN63 SDV61:SDV63 SED61:SED63 SEL61:SEL63 SET61:SET63 SFB61:SFB63 SFJ61:SFJ63 SFR61:SFR63 SFZ61:SFZ63 SGH61:SGH63 SGP61:SGP63 SGX61:SGX63 SHF61:SHF63 SHN61:SHN63 SHV61:SHV63 SID61:SID63 SIL61:SIL63 SIT61:SIT63 SJB61:SJB63 SJJ61:SJJ63 SJR61:SJR63 SJZ61:SJZ63 SKH61:SKH63 SKP61:SKP63 SKX61:SKX63 SLF61:SLF63 SLN61:SLN63 SLV61:SLV63 SMD61:SMD63 SML61:SML63 SMT61:SMT63 SNB61:SNB63 SNJ61:SNJ63 SNR61:SNR63 SNZ61:SNZ63 SOH61:SOH63 SOP61:SOP63 SOX61:SOX63 SPF61:SPF63 SPN61:SPN63 SPV61:SPV63 SQD61:SQD63 SQL61:SQL63 SQT61:SQT63 SRB61:SRB63 SRJ61:SRJ63 SRR61:SRR63 SRZ61:SRZ63 SSH61:SSH63 SSP61:SSP63 SSX61:SSX63 STF61:STF63 STN61:STN63 STV61:STV63 SUD61:SUD63 SUL61:SUL63 SUT61:SUT63 SVB61:SVB63 SVJ61:SVJ63 SVR61:SVR63 SVZ61:SVZ63 SWH61:SWH63 SWP61:SWP63 SWX61:SWX63 SXF61:SXF63 SXN61:SXN63 SXV61:SXV63 SYD61:SYD63 SYL61:SYL63 SYT61:SYT63 SZB61:SZB63 SZJ61:SZJ63 SZR61:SZR63 SZZ61:SZZ63 TAH61:TAH63 TAP61:TAP63 TAX61:TAX63 TBF61:TBF63 TBN61:TBN63 TBV61:TBV63 TCD61:TCD63 TCL61:TCL63 TCT61:TCT63 TDB61:TDB63 TDJ61:TDJ63 TDR61:TDR63 TDZ61:TDZ63 TEH61:TEH63 TEP61:TEP63 TEX61:TEX63 TFF61:TFF63 TFN61:TFN63 TFV61:TFV63 TGD61:TGD63 TGL61:TGL63 TGT61:TGT63 THB61:THB63 THJ61:THJ63 THR61:THR63 THZ61:THZ63 TIH61:TIH63 TIP61:TIP63 TIX61:TIX63 TJF61:TJF63 TJN61:TJN63 TJV61:TJV63 TKD61:TKD63 TKL61:TKL63 TKT61:TKT63 TLB61:TLB63 TLJ61:TLJ63 TLR61:TLR63 TLZ61:TLZ63 TMH61:TMH63 TMP61:TMP63 TMX61:TMX63 TNF61:TNF63 TNN61:TNN63 TNV61:TNV63 TOD61:TOD63 TOL61:TOL63 TOT61:TOT63 TPB61:TPB63 TPJ61:TPJ63 TPR61:TPR63 TPZ61:TPZ63 TQH61:TQH63 TQP61:TQP63 TQX61:TQX63 TRF61:TRF63 TRN61:TRN63 TRV61:TRV63 TSD61:TSD63 TSL61:TSL63 TST61:TST63 TTB61:TTB63 TTJ61:TTJ63 TTR61:TTR63 TTZ61:TTZ63 TUH61:TUH63 TUP61:TUP63 TUX61:TUX63 TVF61:TVF63 TVN61:TVN63 TVV61:TVV63 TWD61:TWD63 TWL61:TWL63 TWT61:TWT63 TXB61:TXB63 TXJ61:TXJ63 TXR61:TXR63 TXZ61:TXZ63 TYH61:TYH63 TYP61:TYP63 TYX61:TYX63 TZF61:TZF63 TZN61:TZN63 TZV61:TZV63 UAD61:UAD63 UAL61:UAL63 UAT61:UAT63 UBB61:UBB63 UBJ61:UBJ63 UBR61:UBR63 UBZ61:UBZ63 UCH61:UCH63 UCP61:UCP63 UCX61:UCX63 UDF61:UDF63 UDN61:UDN63 UDV61:UDV63 UED61:UED63 UEL61:UEL63 UET61:UET63 UFB61:UFB63 UFJ61:UFJ63 UFR61:UFR63 UFZ61:UFZ63 UGH61:UGH63 UGP61:UGP63 UGX61:UGX63 UHF61:UHF63 UHN61:UHN63 UHV61:UHV63 UID61:UID63 UIL61:UIL63 UIT61:UIT63 UJB61:UJB63 UJJ61:UJJ63 UJR61:UJR63 UJZ61:UJZ63 UKH61:UKH63 UKP61:UKP63 UKX61:UKX63 ULF61:ULF63 ULN61:ULN63 ULV61:ULV63 UMD61:UMD63 UML61:UML63 UMT61:UMT63 UNB61:UNB63 UNJ61:UNJ63 UNR61:UNR63 UNZ61:UNZ63 UOH61:UOH63 UOP61:UOP63 UOX61:UOX63 UPF61:UPF63 UPN61:UPN63 UPV61:UPV63 UQD61:UQD63 UQL61:UQL63 UQT61:UQT63 URB61:URB63 URJ61:URJ63 URR61:URR63 URZ61:URZ63 USH61:USH63 USP61:USP63 USX61:USX63 UTF61:UTF63 UTN61:UTN63 UTV61:UTV63 UUD61:UUD63 UUL61:UUL63 UUT61:UUT63 UVB61:UVB63 UVJ61:UVJ63 UVR61:UVR63 UVZ61:UVZ63 UWH61:UWH63 UWP61:UWP63 UWX61:UWX63 UXF61:UXF63 UXN61:UXN63 UXV61:UXV63 UYD61:UYD63 UYL61:UYL63 UYT61:UYT63 UZB61:UZB63 UZJ61:UZJ63 UZR61:UZR63 UZZ61:UZZ63 VAH61:VAH63 VAP61:VAP63 VAX61:VAX63 VBF61:VBF63 VBN61:VBN63 VBV61:VBV63 VCD61:VCD63 VCL61:VCL63 VCT61:VCT63 VDB61:VDB63 VDJ61:VDJ63 VDR61:VDR63 VDZ61:VDZ63 VEH61:VEH63 VEP61:VEP63 VEX61:VEX63 VFF61:VFF63 VFN61:VFN63 VFV61:VFV63 VGD61:VGD63 VGL61:VGL63 VGT61:VGT63 VHB61:VHB63 VHJ61:VHJ63 VHR61:VHR63 VHZ61:VHZ63 VIH61:VIH63 VIP61:VIP63 VIX61:VIX63 VJF61:VJF63 VJN61:VJN63 VJV61:VJV63 VKD61:VKD63 VKL61:VKL63 VKT61:VKT63 VLB61:VLB63 VLJ61:VLJ63 VLR61:VLR63 VLZ61:VLZ63 VMH61:VMH63 VMP61:VMP63 VMX61:VMX63 VNF61:VNF63 VNN61:VNN63 VNV61:VNV63 VOD61:VOD63 VOL61:VOL63 VOT61:VOT63 VPB61:VPB63 VPJ61:VPJ63 VPR61:VPR63 VPZ61:VPZ63 VQH61:VQH63 VQP61:VQP63 VQX61:VQX63 VRF61:VRF63 VRN61:VRN63 VRV61:VRV63 VSD61:VSD63 VSL61:VSL63 VST61:VST63 VTB61:VTB63 VTJ61:VTJ63 VTR61:VTR63 VTZ61:VTZ63 VUH61:VUH63 VUP61:VUP63 VUX61:VUX63 VVF61:VVF63 VVN61:VVN63 VVV61:VVV63 VWD61:VWD63 VWL61:VWL63 VWT61:VWT63 VXB61:VXB63 VXJ61:VXJ63 VXR61:VXR63 VXZ61:VXZ63 VYH61:VYH63 VYP61:VYP63 VYX61:VYX63 VZF61:VZF63 VZN61:VZN63 VZV61:VZV63 WAD61:WAD63 WAL61:WAL63 WAT61:WAT63 WBB61:WBB63 WBJ61:WBJ63 WBR61:WBR63 WBZ61:WBZ63 WCH61:WCH63 WCP61:WCP63 WCX61:WCX63 WDF61:WDF63 WDN61:WDN63 WDV61:WDV63 WED61:WED63 WEL61:WEL63 WET61:WET63 WFB61:WFB63 WFJ61:WFJ63 WFR61:WFR63 WFZ61:WFZ63 WGH61:WGH63 WGP61:WGP63 WGX61:WGX63 WHF61:WHF63 WHN61:WHN63 WHV61:WHV63 WID61:WID63 WIL61:WIL63 WIT61:WIT63 WJB61:WJB63 WJJ61:WJJ63 WJR61:WJR63 WJZ61:WJZ63 WKH61:WKH63 WKP61:WKP63 WKX61:WKX63 WLF61:WLF63 WLN61:WLN63 WLV61:WLV63 WMD61:WMD63 WML61:WML63 WMT61:WMT63 WNB61:WNB63 WNJ61:WNJ63 WNR61:WNR63 WNZ61:WNZ63 WOH61:WOH63 WOP61:WOP63 WOX61:WOX63 WPF61:WPF63 WPN61:WPN63 WPV61:WPV63 WQD61:WQD63 WQL61:WQL63 WQT61:WQT63 WRB61:WRB63 WRJ61:WRJ63 WRR61:WRR63 WRZ61:WRZ63 WSH61:WSH63 WSP61:WSP63 WSX61:WSX63 WTF61:WTF63 WTN61:WTN63 WTV61:WTV63 WUD61:WUD63 WUL61:WUL63 WUT61:WUT63 WVB61:WVB63 WVJ61:WVJ63 WVR61:WVR63 WVZ61:WVZ63 WWH61:WWH63 WWP61:WWP63 WWX61:WWX63 WXF61:WXF63 WXN61:WXN63 WXV61:WXV63 WYD61:WYD63 WYL61:WYL63 WYT61:WYT63 WZB61:WZB63 WZJ61:WZJ63 WZR61:WZR63 WZZ61:WZZ63 XAH61:XAH63 XAP61:XAP63 XAX61:XAX63 XBF61:XBF63 XBN61:XBN63 XBV61:XBV63 XCD61:XCD63 XCL61:XCL63 XCT61:XCT63 XDB61:XDB63 XDJ61:XDJ63 XDR61:XDR63 XDZ61:XDZ63 XEH61:XEH63 XEP61:XEP63 XEX61:XEX63 B68:B69 B3:B66</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>